<commit_message>
Modification of output format
The program results in 5 CVS tables, one for each type of quality
element to be easier to use and more efficient in Power BI.
</commit_message>
<xml_diff>
--- a/Quality metrics and where to find them.xlsx
+++ b/Quality metrics and where to find them.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CCOSSEC\Work Folders\Evaluator configuration\geoe3-quality-dashboard\geoe3-quality-dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312601BE-3BBB-4193-A9E8-44C3F7857019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184DC662-7F5A-4198-BE03-F328F08660C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-13080" yWindow="240" windowWidth="12840" windowHeight="20520" xr2:uid="{D83F700B-A4A3-46DA-B12E-3269EB8805B3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="369">
   <si>
     <t>Type of view</t>
   </si>
@@ -1321,7 +1321,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="59">
+  <borders count="64">
     <border>
       <left/>
       <right/>
@@ -2018,6 +2018,28 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -2032,12 +2054,8 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <right/>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -2045,7 +2063,9 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -2057,10 +2077,39 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -2070,7 +2119,7 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="236">
+  <cellXfs count="243">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2479,9 +2528,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2509,9 +2555,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2536,7 +2579,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="57" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="7" borderId="16" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2710,7 +2753,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2728,10 +2771,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="2" applyBorder="1" applyAlignment="1">
@@ -2741,13 +2784,13 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="50" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="7" borderId="56" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="59" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
@@ -2769,6 +2812,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3219,8 +3289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4480094-795B-499E-8A12-7A8BC9F24E4F}">
   <dimension ref="A1:AB150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E139" sqref="E139"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3325,13 +3395,13 @@
       <c r="S2" s="24"/>
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="175" t="s">
+      <c r="A3" s="173" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="197" t="s">
+      <c r="B3" s="195" t="s">
         <v>307</v>
       </c>
-      <c r="C3" s="221" t="s">
+      <c r="C3" s="219" t="s">
         <v>358</v>
       </c>
       <c r="D3" s="114" t="s">
@@ -3344,14 +3414,14 @@
         <v>143</v>
       </c>
       <c r="G3" s="114"/>
-      <c r="H3" s="153" t="s">
+      <c r="H3" s="151" t="s">
         <v>93</v>
       </c>
       <c r="I3" s="117" t="s">
         <v>359</v>
       </c>
       <c r="J3" s="118"/>
-      <c r="K3" s="215">
+      <c r="K3" s="213">
         <v>3</v>
       </c>
       <c r="L3" s="118"/>
@@ -3367,101 +3437,101 @@
       <c r="T3" s="13"/>
     </row>
     <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="175"/>
-      <c r="B4" s="198"/>
-      <c r="C4" s="212"/>
-      <c r="D4" s="153" t="s">
+      <c r="A4" s="173"/>
+      <c r="B4" s="196"/>
+      <c r="C4" s="210"/>
+      <c r="D4" s="151" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="155"/>
-      <c r="G4" s="153"/>
+      <c r="F4" s="153"/>
+      <c r="G4" s="151"/>
       <c r="H4" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="I4" s="216"/>
-      <c r="J4" s="217"/>
-      <c r="K4" s="218"/>
-      <c r="L4" s="217"/>
-      <c r="M4" s="217"/>
-      <c r="N4" s="216"/>
-      <c r="O4" s="216"/>
-      <c r="P4" s="219"/>
-      <c r="Q4" s="216"/>
-      <c r="R4" s="220"/>
+      <c r="I4" s="214"/>
+      <c r="J4" s="215"/>
+      <c r="K4" s="216"/>
+      <c r="L4" s="215"/>
+      <c r="M4" s="215"/>
+      <c r="N4" s="214"/>
+      <c r="O4" s="214"/>
+      <c r="P4" s="217"/>
+      <c r="Q4" s="214"/>
+      <c r="R4" s="218"/>
       <c r="S4" s="25"/>
       <c r="T4" s="13"/>
     </row>
     <row r="5" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="175"/>
-      <c r="B5" s="198"/>
-      <c r="C5" s="212"/>
-      <c r="D5" s="153" t="s">
+      <c r="A5" s="173"/>
+      <c r="B5" s="196"/>
+      <c r="C5" s="210"/>
+      <c r="D5" s="151" t="s">
         <v>356</v>
       </c>
       <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="155" t="s">
+      <c r="F5" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G5" s="153"/>
-      <c r="H5" s="153" t="s">
+      <c r="G5" s="151"/>
+      <c r="H5" s="151" t="s">
         <v>93</v>
       </c>
-      <c r="I5" s="216" t="s">
+      <c r="I5" s="214" t="s">
         <v>359</v>
       </c>
-      <c r="J5" s="217"/>
-      <c r="K5" s="218"/>
-      <c r="L5" s="217"/>
-      <c r="M5" s="217"/>
-      <c r="N5" s="216"/>
-      <c r="O5" s="216"/>
-      <c r="P5" s="219"/>
-      <c r="Q5" s="216"/>
-      <c r="R5" s="220"/>
+      <c r="J5" s="215"/>
+      <c r="K5" s="216"/>
+      <c r="L5" s="215"/>
+      <c r="M5" s="215"/>
+      <c r="N5" s="214"/>
+      <c r="O5" s="214"/>
+      <c r="P5" s="217"/>
+      <c r="Q5" s="214"/>
+      <c r="R5" s="218"/>
       <c r="S5" s="25"/>
       <c r="T5" s="13"/>
     </row>
     <row r="6" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="175"/>
-      <c r="B6" s="198"/>
-      <c r="C6" s="212"/>
-      <c r="D6" s="153" t="s">
+      <c r="A6" s="173"/>
+      <c r="B6" s="196"/>
+      <c r="C6" s="210"/>
+      <c r="D6" s="151" t="s">
         <v>357</v>
       </c>
       <c r="E6" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="155" t="s">
+      <c r="F6" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G6" s="153"/>
-      <c r="H6" s="153" t="s">
+      <c r="G6" s="151"/>
+      <c r="H6" s="151" t="s">
         <v>93</v>
       </c>
-      <c r="I6" s="216" t="s">
+      <c r="I6" s="214" t="s">
         <v>360</v>
       </c>
-      <c r="J6" s="217"/>
-      <c r="K6" s="218"/>
-      <c r="L6" s="217"/>
-      <c r="M6" s="217"/>
-      <c r="N6" s="216"/>
-      <c r="O6" s="216"/>
-      <c r="P6" s="219"/>
-      <c r="Q6" s="216"/>
-      <c r="R6" s="220"/>
+      <c r="J6" s="215"/>
+      <c r="K6" s="216"/>
+      <c r="L6" s="215"/>
+      <c r="M6" s="215"/>
+      <c r="N6" s="214"/>
+      <c r="O6" s="214"/>
+      <c r="P6" s="217"/>
+      <c r="Q6" s="214"/>
+      <c r="R6" s="218"/>
       <c r="S6" s="25"/>
       <c r="T6" s="13"/>
     </row>
     <row r="7" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="175"/>
-      <c r="B7" s="198"/>
-      <c r="C7" s="213"/>
+      <c r="A7" s="173"/>
+      <c r="B7" s="196"/>
+      <c r="C7" s="211"/>
       <c r="D7" s="41" t="s">
         <v>45</v>
       </c>
@@ -3487,23 +3557,23 @@
       <c r="T7" s="13"/>
     </row>
     <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="175"/>
-      <c r="B8" s="198"/>
-      <c r="C8" s="177" t="s">
+      <c r="A8" s="173"/>
+      <c r="B8" s="196"/>
+      <c r="C8" s="175" t="s">
         <v>343</v>
       </c>
       <c r="D8" s="98" t="s">
         <v>344</v>
       </c>
       <c r="E8" s="46"/>
-      <c r="F8" s="155" t="s">
+      <c r="F8" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G8" s="153"/>
-      <c r="H8" s="153" t="s">
+      <c r="G8" s="151"/>
+      <c r="H8" s="151" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="153"/>
+      <c r="I8" s="151"/>
       <c r="J8" s="53">
         <v>5</v>
       </c>
@@ -3521,21 +3591,21 @@
       <c r="T8" s="13"/>
     </row>
     <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="175"/>
-      <c r="B9" s="198"/>
-      <c r="C9" s="212"/>
+      <c r="A9" s="173"/>
+      <c r="B9" s="196"/>
+      <c r="C9" s="210"/>
       <c r="D9" s="98" t="s">
         <v>345</v>
       </c>
       <c r="E9" s="46"/>
-      <c r="F9" s="155" t="s">
+      <c r="F9" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G9" s="153"/>
-      <c r="H9" s="153" t="s">
+      <c r="G9" s="151"/>
+      <c r="H9" s="151" t="s">
         <v>93</v>
       </c>
-      <c r="I9" s="153"/>
+      <c r="I9" s="151"/>
       <c r="J9" s="53">
         <v>5</v>
       </c>
@@ -3553,21 +3623,21 @@
       <c r="T9" s="13"/>
     </row>
     <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="175"/>
-      <c r="B10" s="198"/>
-      <c r="C10" s="212"/>
+      <c r="A10" s="173"/>
+      <c r="B10" s="196"/>
+      <c r="C10" s="210"/>
       <c r="D10" s="98" t="s">
         <v>346</v>
       </c>
       <c r="E10" s="46"/>
-      <c r="F10" s="155" t="s">
+      <c r="F10" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G10" s="153"/>
-      <c r="H10" s="153" t="s">
+      <c r="G10" s="151"/>
+      <c r="H10" s="151" t="s">
         <v>93</v>
       </c>
-      <c r="I10" s="153"/>
+      <c r="I10" s="151"/>
       <c r="J10" s="53">
         <v>5</v>
       </c>
@@ -3585,21 +3655,21 @@
       <c r="T10" s="13"/>
     </row>
     <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="175"/>
-      <c r="B11" s="198"/>
-      <c r="C11" s="213"/>
+      <c r="A11" s="173"/>
+      <c r="B11" s="196"/>
+      <c r="C11" s="211"/>
       <c r="D11" s="98" t="s">
         <v>347</v>
       </c>
       <c r="E11" s="46"/>
-      <c r="F11" s="155" t="s">
+      <c r="F11" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G11" s="145"/>
-      <c r="H11" s="153" t="s">
+      <c r="G11" s="144"/>
+      <c r="H11" s="151" t="s">
         <v>93</v>
       </c>
-      <c r="I11" s="145"/>
+      <c r="I11" s="144"/>
       <c r="J11" s="53">
         <v>5</v>
       </c>
@@ -3617,38 +3687,38 @@
       <c r="T11" s="13"/>
     </row>
     <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="175"/>
-      <c r="B12" s="198"/>
-      <c r="C12" s="162" t="s">
+      <c r="A12" s="173"/>
+      <c r="B12" s="196"/>
+      <c r="C12" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="162" t="s">
+      <c r="D12" s="160" t="s">
         <v>301</v>
       </c>
-      <c r="E12" s="146" t="s">
+      <c r="E12" s="145" t="s">
         <v>297</v>
       </c>
-      <c r="F12" s="141" t="s">
+      <c r="F12" s="140" t="s">
         <v>143</v>
       </c>
-      <c r="G12" s="145" t="s">
+      <c r="G12" s="144" t="s">
         <v>306</v>
       </c>
-      <c r="H12" s="145" t="s">
+      <c r="H12" s="144" t="s">
         <v>93</v>
       </c>
       <c r="I12" s="35"/>
       <c r="J12" s="36">
         <v>5</v>
       </c>
-      <c r="K12" s="159">
+      <c r="K12" s="157">
         <v>5</v>
       </c>
       <c r="L12" s="36"/>
       <c r="M12" s="36"/>
       <c r="N12" s="35"/>
-      <c r="O12" s="145"/>
-      <c r="P12" s="141"/>
+      <c r="O12" s="144"/>
+      <c r="P12" s="140"/>
       <c r="Q12" s="35" t="s">
         <v>298</v>
       </c>
@@ -3657,32 +3727,32 @@
       <c r="T12" s="13"/>
     </row>
     <row r="13" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="175"/>
-      <c r="B13" s="198"/>
-      <c r="C13" s="174"/>
-      <c r="D13" s="163"/>
-      <c r="E13" s="146" t="s">
+      <c r="A13" s="173"/>
+      <c r="B13" s="196"/>
+      <c r="C13" s="172"/>
+      <c r="D13" s="161"/>
+      <c r="E13" s="145" t="s">
         <v>299</v>
       </c>
-      <c r="F13" s="141" t="s">
+      <c r="F13" s="140" t="s">
         <v>143</v>
       </c>
-      <c r="G13" s="145" t="s">
+      <c r="G13" s="144" t="s">
         <v>305</v>
       </c>
-      <c r="H13" s="145" t="s">
+      <c r="H13" s="144" t="s">
         <v>93</v>
       </c>
       <c r="I13" s="35"/>
       <c r="J13" s="36">
         <v>5</v>
       </c>
-      <c r="K13" s="161"/>
+      <c r="K13" s="159"/>
       <c r="L13" s="36"/>
       <c r="M13" s="36"/>
       <c r="N13" s="35"/>
-      <c r="O13" s="145"/>
-      <c r="P13" s="141"/>
+      <c r="O13" s="144"/>
+      <c r="P13" s="140"/>
       <c r="Q13" s="35" t="s">
         <v>300</v>
       </c>
@@ -3691,22 +3761,22 @@
       <c r="T13" s="13"/>
     </row>
     <row r="14" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="175"/>
-      <c r="B14" s="165"/>
-      <c r="C14" s="174"/>
-      <c r="D14" s="144" t="s">
+      <c r="A14" s="173"/>
+      <c r="B14" s="163"/>
+      <c r="C14" s="172"/>
+      <c r="D14" s="143" t="s">
         <v>302</v>
       </c>
-      <c r="E14" s="146" t="s">
+      <c r="E14" s="145" t="s">
         <v>295</v>
       </c>
-      <c r="F14" s="141" t="s">
+      <c r="F14" s="140" t="s">
         <v>143</v>
       </c>
-      <c r="G14" s="145" t="s">
+      <c r="G14" s="144" t="s">
         <v>304</v>
       </c>
-      <c r="H14" s="145" t="s">
+      <c r="H14" s="144" t="s">
         <v>93</v>
       </c>
       <c r="I14" s="35" t="s">
@@ -3721,8 +3791,8 @@
       <c r="L14" s="36"/>
       <c r="M14" s="36"/>
       <c r="N14" s="35"/>
-      <c r="O14" s="145"/>
-      <c r="P14" s="141"/>
+      <c r="O14" s="144"/>
+      <c r="P14" s="140"/>
       <c r="Q14" s="35" t="s">
         <v>303</v>
       </c>
@@ -3731,8 +3801,8 @@
       <c r="T14" s="13"/>
     </row>
     <row r="15" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="175"/>
-      <c r="B15" s="192" t="s">
+      <c r="A15" s="173"/>
+      <c r="B15" s="190" t="s">
         <v>47</v>
       </c>
       <c r="C15" s="41" t="s">
@@ -3765,8 +3835,8 @@
       <c r="T15" s="13"/>
     </row>
     <row r="16" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="175"/>
-      <c r="B16" s="192"/>
+      <c r="A16" s="173"/>
+      <c r="B16" s="190"/>
       <c r="C16" s="41" t="s">
         <v>48</v>
       </c>
@@ -3795,9 +3865,9 @@
       <c r="T16" s="13"/>
     </row>
     <row r="17" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="175"/>
-      <c r="B17" s="192"/>
-      <c r="C17" s="195" t="s">
+      <c r="A17" s="173"/>
+      <c r="B17" s="190"/>
+      <c r="C17" s="193" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="41" t="s">
@@ -3829,9 +3899,9 @@
       <c r="T17" s="13"/>
     </row>
     <row r="18" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="175"/>
-      <c r="B18" s="192"/>
-      <c r="C18" s="195"/>
+      <c r="A18" s="173"/>
+      <c r="B18" s="190"/>
+      <c r="C18" s="193"/>
       <c r="D18" s="41" t="s">
         <v>50</v>
       </c>
@@ -3861,8 +3931,8 @@
       <c r="T18" s="13"/>
     </row>
     <row r="19" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="175"/>
-      <c r="B19" s="192"/>
+      <c r="A19" s="173"/>
+      <c r="B19" s="190"/>
       <c r="C19" s="41" t="s">
         <v>49</v>
       </c>
@@ -3891,8 +3961,8 @@
       <c r="T19" s="13"/>
     </row>
     <row r="20" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="175"/>
-      <c r="B20" s="192"/>
+      <c r="A20" s="173"/>
+      <c r="B20" s="190"/>
       <c r="C20" s="41" t="s">
         <v>8</v>
       </c>
@@ -3921,11 +3991,11 @@
       <c r="T20" s="13"/>
     </row>
     <row r="21" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="175"/>
-      <c r="B21" s="192" t="s">
+      <c r="A21" s="173"/>
+      <c r="B21" s="190" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="194" t="s">
+      <c r="C21" s="192" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="133" t="s">
@@ -3936,7 +4006,7 @@
       </c>
       <c r="F21" s="49"/>
       <c r="G21" s="41"/>
-      <c r="H21" s="182" t="s">
+      <c r="H21" s="180" t="s">
         <v>296</v>
       </c>
       <c r="I21" s="103"/>
@@ -3957,9 +4027,9 @@
       <c r="T21" s="13"/>
     </row>
     <row r="22" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="175"/>
-      <c r="B22" s="192"/>
-      <c r="C22" s="195"/>
+      <c r="A22" s="173"/>
+      <c r="B22" s="190"/>
+      <c r="C22" s="193"/>
       <c r="D22" s="130" t="s">
         <v>56</v>
       </c>
@@ -3968,7 +4038,7 @@
       </c>
       <c r="F22" s="49"/>
       <c r="G22" s="41"/>
-      <c r="H22" s="183"/>
+      <c r="H22" s="181"/>
       <c r="I22" s="103"/>
       <c r="J22" s="104"/>
       <c r="K22" s="104"/>
@@ -3983,9 +4053,9 @@
       <c r="T22" s="13"/>
     </row>
     <row r="23" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="175"/>
-      <c r="B23" s="192"/>
-      <c r="C23" s="195"/>
+      <c r="A23" s="173"/>
+      <c r="B23" s="190"/>
+      <c r="C23" s="193"/>
       <c r="D23" s="41" t="s">
         <v>57</v>
       </c>
@@ -4013,9 +4083,9 @@
       <c r="T23" s="13"/>
     </row>
     <row r="24" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="175"/>
-      <c r="B24" s="192"/>
-      <c r="C24" s="195" t="s">
+      <c r="A24" s="173"/>
+      <c r="B24" s="190"/>
+      <c r="C24" s="193" t="s">
         <v>11</v>
       </c>
       <c r="D24" s="41" t="s">
@@ -4044,9 +4114,9 @@
       <c r="S24" s="15"/>
     </row>
     <row r="25" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="175"/>
-      <c r="B25" s="192"/>
-      <c r="C25" s="195"/>
+      <c r="A25" s="173"/>
+      <c r="B25" s="190"/>
+      <c r="C25" s="193"/>
       <c r="D25" s="41" t="s">
         <v>50</v>
       </c>
@@ -4073,9 +4143,9 @@
       <c r="S25" s="15"/>
     </row>
     <row r="26" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="175"/>
-      <c r="B26" s="193"/>
-      <c r="C26" s="196"/>
+      <c r="A26" s="173"/>
+      <c r="B26" s="191"/>
+      <c r="C26" s="194"/>
       <c r="D26" s="65" t="s">
         <v>50</v>
       </c>
@@ -4122,16 +4192,16 @@
       <c r="R27" s="109"/>
     </row>
     <row r="28" spans="1:28" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="205" t="s">
+      <c r="A28" s="203" t="s">
         <v>89</v>
       </c>
-      <c r="B28" s="167" t="s">
+      <c r="B28" s="165" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="169" t="s">
+      <c r="C28" s="167" t="s">
         <v>65</v>
       </c>
-      <c r="D28" s="172" t="s">
+      <c r="D28" s="170" t="s">
         <v>39</v>
       </c>
       <c r="E28" s="54" t="s">
@@ -4152,13 +4222,13 @@
       <c r="J28" s="58">
         <v>0</v>
       </c>
-      <c r="K28" s="186">
-        <v>5</v>
-      </c>
-      <c r="L28" s="186">
-        <v>5</v>
-      </c>
-      <c r="M28" s="187" t="s">
+      <c r="K28" s="184">
+        <v>5</v>
+      </c>
+      <c r="L28" s="184">
+        <v>5</v>
+      </c>
+      <c r="M28" s="185" t="s">
         <v>260</v>
       </c>
       <c r="N28" s="57"/>
@@ -4178,10 +4248,10 @@
       <c r="AB28" s="5"/>
     </row>
     <row r="29" spans="1:28" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="205"/>
-      <c r="B29" s="168"/>
-      <c r="C29" s="170"/>
-      <c r="D29" s="173"/>
+      <c r="A29" s="203"/>
+      <c r="B29" s="166"/>
+      <c r="C29" s="168"/>
+      <c r="D29" s="171"/>
       <c r="E29" s="32" t="s">
         <v>186</v>
       </c>
@@ -4200,9 +4270,9 @@
       <c r="J29" s="36">
         <v>0</v>
       </c>
-      <c r="K29" s="180"/>
-      <c r="L29" s="180"/>
-      <c r="M29" s="188"/>
+      <c r="K29" s="178"/>
+      <c r="L29" s="178"/>
+      <c r="M29" s="186"/>
       <c r="N29" s="35"/>
       <c r="O29" s="35"/>
       <c r="P29" s="37"/>
@@ -4220,10 +4290,10 @@
       <c r="AB29" s="7"/>
     </row>
     <row r="30" spans="1:28" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="205"/>
-      <c r="B30" s="168"/>
-      <c r="C30" s="170"/>
-      <c r="D30" s="173"/>
+      <c r="A30" s="203"/>
+      <c r="B30" s="166"/>
+      <c r="C30" s="168"/>
+      <c r="D30" s="171"/>
       <c r="E30" s="32" t="s">
         <v>189</v>
       </c>
@@ -4242,9 +4312,9 @@
       <c r="J30" s="36">
         <v>0</v>
       </c>
-      <c r="K30" s="180"/>
-      <c r="L30" s="180"/>
-      <c r="M30" s="188"/>
+      <c r="K30" s="178"/>
+      <c r="L30" s="178"/>
+      <c r="M30" s="186"/>
       <c r="N30" s="35"/>
       <c r="O30" s="35"/>
       <c r="P30" s="37"/>
@@ -4262,10 +4332,10 @@
       <c r="AB30" s="7"/>
     </row>
     <row r="31" spans="1:28" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="205"/>
-      <c r="B31" s="168"/>
-      <c r="C31" s="170"/>
-      <c r="D31" s="173"/>
+      <c r="A31" s="203"/>
+      <c r="B31" s="166"/>
+      <c r="C31" s="168"/>
+      <c r="D31" s="171"/>
       <c r="E31" s="32" t="s">
         <v>191</v>
       </c>
@@ -4284,9 +4354,9 @@
       <c r="J31" s="36">
         <v>1</v>
       </c>
-      <c r="K31" s="180"/>
-      <c r="L31" s="180"/>
-      <c r="M31" s="188"/>
+      <c r="K31" s="178"/>
+      <c r="L31" s="178"/>
+      <c r="M31" s="186"/>
       <c r="N31" s="35"/>
       <c r="O31" s="35"/>
       <c r="P31" s="37"/>
@@ -4304,10 +4374,10 @@
       <c r="AB31" s="7"/>
     </row>
     <row r="32" spans="1:28" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="205"/>
-      <c r="B32" s="168"/>
-      <c r="C32" s="170"/>
-      <c r="D32" s="173"/>
+      <c r="A32" s="203"/>
+      <c r="B32" s="166"/>
+      <c r="C32" s="168"/>
+      <c r="D32" s="171"/>
       <c r="E32" s="32" t="s">
         <v>194</v>
       </c>
@@ -4326,9 +4396,9 @@
       <c r="J32" s="36">
         <v>1</v>
       </c>
-      <c r="K32" s="180"/>
-      <c r="L32" s="180"/>
-      <c r="M32" s="188"/>
+      <c r="K32" s="178"/>
+      <c r="L32" s="178"/>
+      <c r="M32" s="186"/>
       <c r="N32" s="35"/>
       <c r="O32" s="35"/>
       <c r="P32" s="37"/>
@@ -4346,10 +4416,10 @@
       <c r="AB32" s="7"/>
     </row>
     <row r="33" spans="1:28" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="205"/>
-      <c r="B33" s="168"/>
-      <c r="C33" s="170"/>
-      <c r="D33" s="173"/>
+      <c r="A33" s="203"/>
+      <c r="B33" s="166"/>
+      <c r="C33" s="168"/>
+      <c r="D33" s="171"/>
       <c r="E33" s="32" t="s">
         <v>195</v>
       </c>
@@ -4368,9 +4438,9 @@
       <c r="J33" s="36">
         <v>1</v>
       </c>
-      <c r="K33" s="180"/>
-      <c r="L33" s="180"/>
-      <c r="M33" s="188"/>
+      <c r="K33" s="178"/>
+      <c r="L33" s="178"/>
+      <c r="M33" s="186"/>
       <c r="N33" s="35"/>
       <c r="O33" s="35"/>
       <c r="P33" s="37"/>
@@ -4388,10 +4458,10 @@
       <c r="AB33" s="7"/>
     </row>
     <row r="34" spans="1:28" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="205"/>
-      <c r="B34" s="168"/>
-      <c r="C34" s="170"/>
-      <c r="D34" s="173"/>
+      <c r="A34" s="203"/>
+      <c r="B34" s="166"/>
+      <c r="C34" s="168"/>
+      <c r="D34" s="171"/>
       <c r="E34" s="32" t="s">
         <v>196</v>
       </c>
@@ -4410,9 +4480,9 @@
       <c r="J34" s="36">
         <v>8</v>
       </c>
-      <c r="K34" s="180"/>
-      <c r="L34" s="180"/>
-      <c r="M34" s="188"/>
+      <c r="K34" s="178"/>
+      <c r="L34" s="178"/>
+      <c r="M34" s="186"/>
       <c r="N34" s="35"/>
       <c r="O34" s="35"/>
       <c r="P34" s="37"/>
@@ -4430,10 +4500,10 @@
       <c r="AB34" s="7"/>
     </row>
     <row r="35" spans="1:28" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="205"/>
-      <c r="B35" s="168"/>
-      <c r="C35" s="170"/>
-      <c r="D35" s="173"/>
+      <c r="A35" s="203"/>
+      <c r="B35" s="166"/>
+      <c r="C35" s="168"/>
+      <c r="D35" s="171"/>
       <c r="E35" s="32" t="s">
         <v>200</v>
       </c>
@@ -4452,9 +4522,9 @@
       <c r="J35" s="36">
         <v>4</v>
       </c>
-      <c r="K35" s="180"/>
-      <c r="L35" s="180"/>
-      <c r="M35" s="188"/>
+      <c r="K35" s="178"/>
+      <c r="L35" s="178"/>
+      <c r="M35" s="186"/>
       <c r="N35" s="35"/>
       <c r="O35" s="35"/>
       <c r="P35" s="37"/>
@@ -4472,10 +4542,10 @@
       <c r="AB35" s="7"/>
     </row>
     <row r="36" spans="1:28" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="205"/>
-      <c r="B36" s="168"/>
-      <c r="C36" s="170"/>
-      <c r="D36" s="173"/>
+      <c r="A36" s="203"/>
+      <c r="B36" s="166"/>
+      <c r="C36" s="168"/>
+      <c r="D36" s="171"/>
       <c r="E36" s="32" t="s">
         <v>201</v>
       </c>
@@ -4494,9 +4564,9 @@
       <c r="J36" s="36">
         <v>4</v>
       </c>
-      <c r="K36" s="180"/>
-      <c r="L36" s="180"/>
-      <c r="M36" s="188"/>
+      <c r="K36" s="178"/>
+      <c r="L36" s="178"/>
+      <c r="M36" s="186"/>
       <c r="N36" s="35"/>
       <c r="O36" s="35"/>
       <c r="P36" s="37"/>
@@ -4514,10 +4584,10 @@
       <c r="AB36" s="7"/>
     </row>
     <row r="37" spans="1:28" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="205"/>
-      <c r="B37" s="168"/>
-      <c r="C37" s="170"/>
-      <c r="D37" s="173"/>
+      <c r="A37" s="203"/>
+      <c r="B37" s="166"/>
+      <c r="C37" s="168"/>
+      <c r="D37" s="171"/>
       <c r="E37" s="32" t="s">
         <v>202</v>
       </c>
@@ -4536,9 +4606,9 @@
       <c r="J37" s="36">
         <v>4</v>
       </c>
-      <c r="K37" s="180"/>
-      <c r="L37" s="180"/>
-      <c r="M37" s="188"/>
+      <c r="K37" s="178"/>
+      <c r="L37" s="178"/>
+      <c r="M37" s="186"/>
       <c r="N37" s="35"/>
       <c r="O37" s="35"/>
       <c r="P37" s="37"/>
@@ -4556,10 +4626,10 @@
       <c r="AB37" s="7"/>
     </row>
     <row r="38" spans="1:28" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="205"/>
-      <c r="B38" s="168"/>
-      <c r="C38" s="170"/>
-      <c r="D38" s="173"/>
+      <c r="A38" s="203"/>
+      <c r="B38" s="166"/>
+      <c r="C38" s="168"/>
+      <c r="D38" s="171"/>
       <c r="E38" s="32" t="s">
         <v>205</v>
       </c>
@@ -4578,9 +4648,9 @@
       <c r="J38" s="36">
         <v>4</v>
       </c>
-      <c r="K38" s="180"/>
-      <c r="L38" s="180"/>
-      <c r="M38" s="188"/>
+      <c r="K38" s="178"/>
+      <c r="L38" s="178"/>
+      <c r="M38" s="186"/>
       <c r="N38" s="35"/>
       <c r="O38" s="35"/>
       <c r="P38" s="37"/>
@@ -4598,10 +4668,10 @@
       <c r="AB38" s="7"/>
     </row>
     <row r="39" spans="1:28" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="205"/>
-      <c r="B39" s="168"/>
-      <c r="C39" s="170"/>
-      <c r="D39" s="173"/>
+      <c r="A39" s="203"/>
+      <c r="B39" s="166"/>
+      <c r="C39" s="168"/>
+      <c r="D39" s="171"/>
       <c r="E39" s="32" t="s">
         <v>207</v>
       </c>
@@ -4620,9 +4690,9 @@
       <c r="J39" s="36">
         <v>4</v>
       </c>
-      <c r="K39" s="180"/>
-      <c r="L39" s="180"/>
-      <c r="M39" s="188"/>
+      <c r="K39" s="178"/>
+      <c r="L39" s="178"/>
+      <c r="M39" s="186"/>
       <c r="N39" s="35"/>
       <c r="O39" s="35"/>
       <c r="P39" s="37"/>
@@ -4640,10 +4710,10 @@
       <c r="AB39" s="7"/>
     </row>
     <row r="40" spans="1:28" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="205"/>
-      <c r="B40" s="168"/>
-      <c r="C40" s="170"/>
-      <c r="D40" s="173"/>
+      <c r="A40" s="203"/>
+      <c r="B40" s="166"/>
+      <c r="C40" s="168"/>
+      <c r="D40" s="171"/>
       <c r="E40" s="32" t="s">
         <v>211</v>
       </c>
@@ -4662,9 +4732,9 @@
       <c r="J40" s="36">
         <v>0</v>
       </c>
-      <c r="K40" s="180"/>
-      <c r="L40" s="180"/>
-      <c r="M40" s="188"/>
+      <c r="K40" s="178"/>
+      <c r="L40" s="178"/>
+      <c r="M40" s="186"/>
       <c r="N40" s="35"/>
       <c r="O40" s="35"/>
       <c r="P40" s="37"/>
@@ -4682,10 +4752,10 @@
       <c r="AB40" s="7"/>
     </row>
     <row r="41" spans="1:28" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="205"/>
-      <c r="B41" s="168"/>
-      <c r="C41" s="170"/>
-      <c r="D41" s="173"/>
+      <c r="A41" s="203"/>
+      <c r="B41" s="166"/>
+      <c r="C41" s="168"/>
+      <c r="D41" s="171"/>
       <c r="E41" s="32" t="s">
         <v>212</v>
       </c>
@@ -4704,9 +4774,9 @@
       <c r="J41" s="36">
         <v>0</v>
       </c>
-      <c r="K41" s="180"/>
-      <c r="L41" s="180"/>
-      <c r="M41" s="188"/>
+      <c r="K41" s="178"/>
+      <c r="L41" s="178"/>
+      <c r="M41" s="186"/>
       <c r="N41" s="35"/>
       <c r="O41" s="35"/>
       <c r="P41" s="37"/>
@@ -4724,10 +4794,10 @@
       <c r="AB41" s="7"/>
     </row>
     <row r="42" spans="1:28" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="205"/>
-      <c r="B42" s="168"/>
-      <c r="C42" s="170"/>
-      <c r="D42" s="173"/>
+      <c r="A42" s="203"/>
+      <c r="B42" s="166"/>
+      <c r="C42" s="168"/>
+      <c r="D42" s="171"/>
       <c r="E42" s="32" t="s">
         <v>213</v>
       </c>
@@ -4746,9 +4816,9 @@
       <c r="J42" s="36">
         <v>0</v>
       </c>
-      <c r="K42" s="180"/>
-      <c r="L42" s="180"/>
-      <c r="M42" s="188"/>
+      <c r="K42" s="178"/>
+      <c r="L42" s="178"/>
+      <c r="M42" s="186"/>
       <c r="N42" s="35"/>
       <c r="O42" s="35"/>
       <c r="P42" s="37"/>
@@ -4766,11 +4836,11 @@
       <c r="AB42" s="7"/>
     </row>
     <row r="43" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="205"/>
-      <c r="B43" s="168" t="s">
+      <c r="A43" s="203"/>
+      <c r="B43" s="166" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="170" t="s">
+      <c r="C43" s="168" t="s">
         <v>16</v>
       </c>
       <c r="D43" s="39" t="s">
@@ -4794,13 +4864,13 @@
       <c r="J43" s="42">
         <v>5</v>
       </c>
-      <c r="K43" s="184">
-        <v>5</v>
-      </c>
-      <c r="L43" s="184">
-        <v>5</v>
-      </c>
-      <c r="M43" s="184">
+      <c r="K43" s="182">
+        <v>5</v>
+      </c>
+      <c r="L43" s="182">
+        <v>5</v>
+      </c>
+      <c r="M43" s="182">
         <v>5</v>
       </c>
       <c r="N43" s="43"/>
@@ -4815,9 +4885,9 @@
       <c r="S43" s="26"/>
     </row>
     <row r="44" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="205"/>
-      <c r="B44" s="168"/>
-      <c r="C44" s="170"/>
+      <c r="A44" s="203"/>
+      <c r="B44" s="166"/>
+      <c r="C44" s="168"/>
       <c r="D44" s="39" t="s">
         <v>17</v>
       </c>
@@ -4839,9 +4909,9 @@
       <c r="J44" s="42">
         <v>1</v>
       </c>
-      <c r="K44" s="184"/>
-      <c r="L44" s="184"/>
-      <c r="M44" s="184"/>
+      <c r="K44" s="182"/>
+      <c r="L44" s="182"/>
+      <c r="M44" s="182"/>
       <c r="N44" s="43"/>
       <c r="O44" s="35"/>
       <c r="P44" s="37"/>
@@ -4854,9 +4924,9 @@
       <c r="S44" s="26"/>
     </row>
     <row r="45" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="205"/>
-      <c r="B45" s="168"/>
-      <c r="C45" s="170"/>
+      <c r="A45" s="203"/>
+      <c r="B45" s="166"/>
+      <c r="C45" s="168"/>
       <c r="D45" s="39" t="s">
         <v>17</v>
       </c>
@@ -4878,9 +4948,9 @@
       <c r="J45" s="42">
         <v>7</v>
       </c>
-      <c r="K45" s="184"/>
-      <c r="L45" s="184"/>
-      <c r="M45" s="184"/>
+      <c r="K45" s="182"/>
+      <c r="L45" s="182"/>
+      <c r="M45" s="182"/>
       <c r="N45" s="43"/>
       <c r="O45" s="35"/>
       <c r="P45" s="37"/>
@@ -4889,9 +4959,9 @@
       <c r="S45" s="26"/>
     </row>
     <row r="46" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="205"/>
-      <c r="B46" s="168"/>
-      <c r="C46" s="170"/>
+      <c r="A46" s="203"/>
+      <c r="B46" s="166"/>
+      <c r="C46" s="168"/>
       <c r="D46" s="52" t="s">
         <v>215</v>
       </c>
@@ -4912,8 +4982,8 @@
       <c r="K46" s="36">
         <v>7</v>
       </c>
-      <c r="L46" s="184"/>
-      <c r="M46" s="184"/>
+      <c r="L46" s="182"/>
+      <c r="M46" s="182"/>
       <c r="N46" s="41"/>
       <c r="O46" s="41"/>
       <c r="P46" s="37"/>
@@ -4926,9 +4996,9 @@
       <c r="S46" s="26"/>
     </row>
     <row r="47" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="205"/>
-      <c r="B47" s="168"/>
-      <c r="C47" s="170" t="s">
+      <c r="A47" s="203"/>
+      <c r="B47" s="166"/>
+      <c r="C47" s="168" t="s">
         <v>218</v>
       </c>
       <c r="D47" s="39" t="s">
@@ -4955,10 +5025,10 @@
       <c r="K47" s="42">
         <v>2</v>
       </c>
-      <c r="L47" s="184">
-        <v>5</v>
-      </c>
-      <c r="M47" s="184"/>
+      <c r="L47" s="182">
+        <v>5</v>
+      </c>
+      <c r="M47" s="182"/>
       <c r="N47" s="43"/>
       <c r="O47" s="35"/>
       <c r="P47" s="37"/>
@@ -4971,9 +5041,9 @@
       <c r="S47" s="26"/>
     </row>
     <row r="48" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="205"/>
-      <c r="B48" s="168"/>
-      <c r="C48" s="170"/>
+      <c r="A48" s="203"/>
+      <c r="B48" s="166"/>
+      <c r="C48" s="168"/>
       <c r="D48" s="52" t="s">
         <v>217</v>
       </c>
@@ -4994,8 +5064,8 @@
       <c r="K48" s="42">
         <v>7</v>
       </c>
-      <c r="L48" s="184"/>
-      <c r="M48" s="184"/>
+      <c r="L48" s="182"/>
+      <c r="M48" s="182"/>
       <c r="N48" s="43"/>
       <c r="O48" s="35" t="s">
         <v>219</v>
@@ -5006,9 +5076,9 @@
       <c r="S48" s="26"/>
     </row>
     <row r="49" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="205"/>
-      <c r="B49" s="168"/>
-      <c r="C49" s="170"/>
+      <c r="A49" s="203"/>
+      <c r="B49" s="166"/>
+      <c r="C49" s="168"/>
       <c r="D49" s="39" t="s">
         <v>15</v>
       </c>
@@ -5030,11 +5100,11 @@
       <c r="J49" s="42">
         <v>5</v>
       </c>
-      <c r="K49" s="184">
-        <v>5</v>
-      </c>
-      <c r="L49" s="184"/>
-      <c r="M49" s="184"/>
+      <c r="K49" s="182">
+        <v>5</v>
+      </c>
+      <c r="L49" s="182"/>
+      <c r="M49" s="182"/>
       <c r="N49" s="43"/>
       <c r="O49" s="35"/>
       <c r="P49" s="37"/>
@@ -5047,9 +5117,9 @@
       <c r="S49" s="26"/>
     </row>
     <row r="50" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="205"/>
-      <c r="B50" s="168"/>
-      <c r="C50" s="170"/>
+      <c r="A50" s="203"/>
+      <c r="B50" s="166"/>
+      <c r="C50" s="168"/>
       <c r="D50" s="39" t="s">
         <v>15</v>
       </c>
@@ -5071,9 +5141,9 @@
       <c r="J50" s="42">
         <v>1</v>
       </c>
-      <c r="K50" s="184"/>
-      <c r="L50" s="184"/>
-      <c r="M50" s="184"/>
+      <c r="K50" s="182"/>
+      <c r="L50" s="182"/>
+      <c r="M50" s="182"/>
       <c r="N50" s="43"/>
       <c r="O50" s="35"/>
       <c r="P50" s="37"/>
@@ -5086,9 +5156,9 @@
       <c r="S50" s="26"/>
     </row>
     <row r="51" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="205"/>
-      <c r="B51" s="168"/>
-      <c r="C51" s="170"/>
+      <c r="A51" s="203"/>
+      <c r="B51" s="166"/>
+      <c r="C51" s="168"/>
       <c r="D51" s="39" t="s">
         <v>15</v>
       </c>
@@ -5110,9 +5180,9 @@
       <c r="J51" s="42">
         <v>7</v>
       </c>
-      <c r="K51" s="184"/>
-      <c r="L51" s="184"/>
-      <c r="M51" s="184"/>
+      <c r="K51" s="182"/>
+      <c r="L51" s="182"/>
+      <c r="M51" s="182"/>
       <c r="N51" s="43"/>
       <c r="O51" s="35"/>
       <c r="P51" s="37"/>
@@ -5125,11 +5195,11 @@
       <c r="S51" s="26"/>
     </row>
     <row r="52" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="205"/>
-      <c r="B52" s="168" t="s">
+      <c r="A52" s="203"/>
+      <c r="B52" s="166" t="s">
         <v>18</v>
       </c>
-      <c r="C52" s="170" t="s">
+      <c r="C52" s="168" t="s">
         <v>138</v>
       </c>
       <c r="D52" s="39" t="s">
@@ -5156,10 +5226,10 @@
       <c r="K52" s="42">
         <v>8</v>
       </c>
-      <c r="L52" s="184">
+      <c r="L52" s="182">
         <v>7</v>
       </c>
-      <c r="M52" s="184">
+      <c r="M52" s="182">
         <v>5</v>
       </c>
       <c r="N52" s="43"/>
@@ -5172,9 +5242,9 @@
       <c r="S52" s="26"/>
     </row>
     <row r="53" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="205"/>
-      <c r="B53" s="168"/>
-      <c r="C53" s="170"/>
+      <c r="A53" s="203"/>
+      <c r="B53" s="166"/>
+      <c r="C53" s="168"/>
       <c r="D53" s="39" t="s">
         <v>72</v>
       </c>
@@ -5196,11 +5266,11 @@
       <c r="J53" s="42">
         <v>7</v>
       </c>
-      <c r="K53" s="184">
-        <v>5</v>
-      </c>
-      <c r="L53" s="184"/>
-      <c r="M53" s="184"/>
+      <c r="K53" s="182">
+        <v>5</v>
+      </c>
+      <c r="L53" s="182"/>
+      <c r="M53" s="182"/>
       <c r="N53" s="43"/>
       <c r="O53" s="35"/>
       <c r="P53" s="37"/>
@@ -5213,9 +5283,9 @@
       <c r="S53" s="26"/>
     </row>
     <row r="54" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="205"/>
-      <c r="B54" s="168"/>
-      <c r="C54" s="170"/>
+      <c r="A54" s="203"/>
+      <c r="B54" s="166"/>
+      <c r="C54" s="168"/>
       <c r="D54" s="39" t="s">
         <v>70</v>
       </c>
@@ -5237,9 +5307,9 @@
       <c r="J54" s="42">
         <v>1</v>
       </c>
-      <c r="K54" s="184"/>
-      <c r="L54" s="184"/>
-      <c r="M54" s="184"/>
+      <c r="K54" s="182"/>
+      <c r="L54" s="182"/>
+      <c r="M54" s="182"/>
       <c r="N54" s="43"/>
       <c r="O54" s="35"/>
       <c r="P54" s="37"/>
@@ -5252,9 +5322,9 @@
       <c r="S54" s="26"/>
     </row>
     <row r="55" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="205"/>
-      <c r="B55" s="168"/>
-      <c r="C55" s="170" t="s">
+      <c r="A55" s="203"/>
+      <c r="B55" s="166"/>
+      <c r="C55" s="168" t="s">
         <v>19</v>
       </c>
       <c r="D55" s="39" t="s">
@@ -5281,10 +5351,10 @@
       <c r="K55" s="42">
         <v>8</v>
       </c>
-      <c r="L55" s="184">
+      <c r="L55" s="182">
         <v>7</v>
       </c>
-      <c r="M55" s="184"/>
+      <c r="M55" s="182"/>
       <c r="N55" s="43"/>
       <c r="O55" s="35"/>
       <c r="P55" s="37"/>
@@ -5295,9 +5365,9 @@
       <c r="S55" s="26"/>
     </row>
     <row r="56" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="205"/>
-      <c r="B56" s="168"/>
-      <c r="C56" s="170"/>
+      <c r="A56" s="203"/>
+      <c r="B56" s="166"/>
+      <c r="C56" s="168"/>
       <c r="D56" s="39" t="s">
         <v>72</v>
       </c>
@@ -5319,11 +5389,11 @@
       <c r="J56" s="42">
         <v>7</v>
       </c>
-      <c r="K56" s="184">
-        <v>5</v>
-      </c>
-      <c r="L56" s="184"/>
-      <c r="M56" s="184"/>
+      <c r="K56" s="182">
+        <v>5</v>
+      </c>
+      <c r="L56" s="182"/>
+      <c r="M56" s="182"/>
       <c r="N56" s="43"/>
       <c r="O56" s="35"/>
       <c r="P56" s="37"/>
@@ -5336,9 +5406,9 @@
       <c r="S56" s="26"/>
     </row>
     <row r="57" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="205"/>
-      <c r="B57" s="168"/>
-      <c r="C57" s="191"/>
+      <c r="A57" s="203"/>
+      <c r="B57" s="166"/>
+      <c r="C57" s="189"/>
       <c r="D57" s="39" t="s">
         <v>70</v>
       </c>
@@ -5360,9 +5430,9 @@
       <c r="J57" s="42">
         <v>1</v>
       </c>
-      <c r="K57" s="184"/>
-      <c r="L57" s="184"/>
-      <c r="M57" s="184"/>
+      <c r="K57" s="182"/>
+      <c r="L57" s="182"/>
+      <c r="M57" s="182"/>
       <c r="N57" s="43"/>
       <c r="O57" s="35"/>
       <c r="P57" s="37"/>
@@ -5375,9 +5445,9 @@
       <c r="S57" s="26"/>
     </row>
     <row r="58" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="205"/>
-      <c r="B58" s="189"/>
-      <c r="C58" s="170" t="s">
+      <c r="A58" s="203"/>
+      <c r="B58" s="187"/>
+      <c r="C58" s="168" t="s">
         <v>20</v>
       </c>
       <c r="D58" s="112" t="s">
@@ -5404,10 +5474,10 @@
       <c r="K58" s="42">
         <v>8</v>
       </c>
-      <c r="L58" s="184">
+      <c r="L58" s="182">
         <v>7</v>
       </c>
-      <c r="M58" s="184"/>
+      <c r="M58" s="182"/>
       <c r="N58" s="43"/>
       <c r="O58" s="35"/>
       <c r="P58" s="37"/>
@@ -5418,9 +5488,9 @@
       <c r="S58" s="26"/>
     </row>
     <row r="59" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="205"/>
-      <c r="B59" s="189"/>
-      <c r="C59" s="170"/>
+      <c r="A59" s="203"/>
+      <c r="B59" s="187"/>
+      <c r="C59" s="168"/>
       <c r="D59" s="112" t="s">
         <v>128</v>
       </c>
@@ -5442,11 +5512,11 @@
       <c r="J59" s="42">
         <v>5</v>
       </c>
-      <c r="K59" s="184">
-        <v>5</v>
-      </c>
-      <c r="L59" s="184"/>
-      <c r="M59" s="184"/>
+      <c r="K59" s="182">
+        <v>5</v>
+      </c>
+      <c r="L59" s="182"/>
+      <c r="M59" s="182"/>
       <c r="N59" s="43"/>
       <c r="O59" s="35"/>
       <c r="P59" s="37"/>
@@ -5459,9 +5529,9 @@
       <c r="S59" s="26"/>
     </row>
     <row r="60" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="205"/>
-      <c r="B60" s="189"/>
-      <c r="C60" s="170"/>
+      <c r="A60" s="203"/>
+      <c r="B60" s="187"/>
+      <c r="C60" s="168"/>
       <c r="D60" s="112" t="s">
         <v>128</v>
       </c>
@@ -5483,9 +5553,9 @@
       <c r="J60" s="42">
         <v>5</v>
       </c>
-      <c r="K60" s="184"/>
-      <c r="L60" s="184"/>
-      <c r="M60" s="184"/>
+      <c r="K60" s="182"/>
+      <c r="L60" s="182"/>
+      <c r="M60" s="182"/>
       <c r="N60" s="43"/>
       <c r="O60" s="35"/>
       <c r="P60" s="37"/>
@@ -5498,11 +5568,11 @@
       <c r="S60" s="26"/>
     </row>
     <row r="61" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="205"/>
-      <c r="B61" s="171" t="s">
+      <c r="A61" s="203"/>
+      <c r="B61" s="169" t="s">
         <v>73</v>
       </c>
-      <c r="C61" s="203" t="s">
+      <c r="C61" s="201" t="s">
         <v>21</v>
       </c>
       <c r="D61" s="39" t="s">
@@ -5524,13 +5594,13 @@
       <c r="J61" s="47">
         <v>5</v>
       </c>
-      <c r="K61" s="185">
+      <c r="K61" s="183">
         <v>7</v>
       </c>
-      <c r="L61" s="185">
+      <c r="L61" s="183">
         <v>6</v>
       </c>
-      <c r="M61" s="178">
+      <c r="M61" s="176">
         <v>5</v>
       </c>
       <c r="N61" s="35"/>
@@ -5541,9 +5611,9 @@
       <c r="S61" s="26"/>
     </row>
     <row r="62" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="205"/>
-      <c r="B62" s="171"/>
-      <c r="C62" s="204"/>
+      <c r="A62" s="203"/>
+      <c r="B62" s="169"/>
+      <c r="C62" s="202"/>
       <c r="D62" s="39" t="s">
         <v>250</v>
       </c>
@@ -5563,9 +5633,9 @@
       <c r="J62" s="47">
         <v>5</v>
       </c>
-      <c r="K62" s="185"/>
-      <c r="L62" s="185"/>
-      <c r="M62" s="178"/>
+      <c r="K62" s="183"/>
+      <c r="L62" s="183"/>
+      <c r="M62" s="176"/>
       <c r="N62" s="35"/>
       <c r="O62" s="41"/>
       <c r="P62" s="48"/>
@@ -5574,9 +5644,9 @@
       <c r="S62" s="26"/>
     </row>
     <row r="63" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="205"/>
-      <c r="B63" s="171"/>
-      <c r="C63" s="204"/>
+      <c r="A63" s="203"/>
+      <c r="B63" s="169"/>
+      <c r="C63" s="202"/>
       <c r="D63" s="39" t="s">
         <v>251</v>
       </c>
@@ -5599,8 +5669,8 @@
       <c r="K63" s="47">
         <v>5</v>
       </c>
-      <c r="L63" s="185"/>
-      <c r="M63" s="178"/>
+      <c r="L63" s="183"/>
+      <c r="M63" s="176"/>
       <c r="N63" s="35"/>
       <c r="O63" s="45"/>
       <c r="P63" s="48"/>
@@ -5609,9 +5679,9 @@
       <c r="S63" s="26"/>
     </row>
     <row r="64" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="205"/>
-      <c r="B64" s="171"/>
-      <c r="C64" s="204"/>
+      <c r="A64" s="203"/>
+      <c r="B64" s="169"/>
+      <c r="C64" s="202"/>
       <c r="D64" s="39" t="s">
         <v>252</v>
       </c>
@@ -5634,8 +5704,8 @@
       <c r="K64" s="47">
         <v>5</v>
       </c>
-      <c r="L64" s="185"/>
-      <c r="M64" s="178"/>
+      <c r="L64" s="183"/>
+      <c r="M64" s="176"/>
       <c r="N64" s="35"/>
       <c r="O64" s="45"/>
       <c r="P64" s="48"/>
@@ -5644,8 +5714,8 @@
       <c r="S64" s="26"/>
     </row>
     <row r="65" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="205"/>
-      <c r="B65" s="171"/>
+      <c r="A65" s="203"/>
+      <c r="B65" s="169"/>
       <c r="C65" s="39" t="s">
         <v>22</v>
       </c>
@@ -5676,7 +5746,7 @@
       <c r="L65" s="47">
         <v>5</v>
       </c>
-      <c r="M65" s="178"/>
+      <c r="M65" s="176"/>
       <c r="N65" s="35"/>
       <c r="O65" s="34"/>
       <c r="P65" s="33"/>
@@ -5685,9 +5755,9 @@
       <c r="S65" s="15"/>
     </row>
     <row r="66" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="205"/>
-      <c r="B66" s="171"/>
-      <c r="C66" s="204" t="s">
+      <c r="A66" s="203"/>
+      <c r="B66" s="169"/>
+      <c r="C66" s="202" t="s">
         <v>23</v>
       </c>
       <c r="D66" s="39" t="s">
@@ -5714,10 +5784,10 @@
       <c r="K66" s="47">
         <v>5</v>
       </c>
-      <c r="L66" s="185">
+      <c r="L66" s="183">
         <v>8</v>
       </c>
-      <c r="M66" s="178"/>
+      <c r="M66" s="176"/>
       <c r="N66" s="35"/>
       <c r="O66" s="38" t="s">
         <v>222</v>
@@ -5728,9 +5798,9 @@
       <c r="S66" s="15"/>
     </row>
     <row r="67" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="205"/>
-      <c r="B67" s="171"/>
-      <c r="C67" s="204"/>
+      <c r="A67" s="203"/>
+      <c r="B67" s="169"/>
+      <c r="C67" s="202"/>
       <c r="D67" s="39" t="s">
         <v>221</v>
       </c>
@@ -5755,8 +5825,8 @@
       <c r="K67" s="47">
         <v>5</v>
       </c>
-      <c r="L67" s="185"/>
-      <c r="M67" s="178"/>
+      <c r="L67" s="183"/>
+      <c r="M67" s="176"/>
       <c r="N67" s="41"/>
       <c r="O67" s="38" t="s">
         <v>223</v>
@@ -5767,9 +5837,9 @@
       <c r="S67" s="15"/>
     </row>
     <row r="68" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="205"/>
-      <c r="B68" s="171"/>
-      <c r="C68" s="204"/>
+      <c r="A68" s="203"/>
+      <c r="B68" s="169"/>
+      <c r="C68" s="202"/>
       <c r="D68" s="39" t="s">
         <v>224</v>
       </c>
@@ -5794,8 +5864,8 @@
       <c r="K68" s="47">
         <v>5</v>
       </c>
-      <c r="L68" s="185"/>
-      <c r="M68" s="178"/>
+      <c r="L68" s="183"/>
+      <c r="M68" s="176"/>
       <c r="N68" s="41"/>
       <c r="O68" s="38" t="s">
         <v>223</v>
@@ -5806,9 +5876,9 @@
       <c r="S68" s="15"/>
     </row>
     <row r="69" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="205"/>
-      <c r="B69" s="171"/>
-      <c r="C69" s="158" t="s">
+      <c r="A69" s="203"/>
+      <c r="B69" s="169"/>
+      <c r="C69" s="156" t="s">
         <v>239</v>
       </c>
       <c r="D69" s="39" t="s">
@@ -5835,10 +5905,10 @@
       <c r="K69" s="47">
         <v>5</v>
       </c>
-      <c r="L69" s="185">
-        <v>5</v>
-      </c>
-      <c r="M69" s="178"/>
+      <c r="L69" s="183">
+        <v>5</v>
+      </c>
+      <c r="M69" s="176"/>
       <c r="N69" s="41"/>
       <c r="O69" s="38"/>
       <c r="P69" s="33"/>
@@ -5847,9 +5917,9 @@
       <c r="S69" s="15"/>
     </row>
     <row r="70" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="205"/>
-      <c r="B70" s="171"/>
-      <c r="C70" s="158"/>
+      <c r="A70" s="203"/>
+      <c r="B70" s="169"/>
+      <c r="C70" s="156"/>
       <c r="D70" s="39" t="s">
         <v>245</v>
       </c>
@@ -5874,8 +5944,8 @@
       <c r="K70" s="47">
         <v>5</v>
       </c>
-      <c r="L70" s="185"/>
-      <c r="M70" s="178"/>
+      <c r="L70" s="183"/>
+      <c r="M70" s="176"/>
       <c r="N70" s="41"/>
       <c r="O70" s="38"/>
       <c r="P70" s="33"/>
@@ -5884,9 +5954,9 @@
       <c r="S70" s="15"/>
     </row>
     <row r="71" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="205"/>
-      <c r="B71" s="171"/>
-      <c r="C71" s="158"/>
+      <c r="A71" s="203"/>
+      <c r="B71" s="169"/>
+      <c r="C71" s="156"/>
       <c r="D71" s="39" t="s">
         <v>246</v>
       </c>
@@ -5911,8 +5981,8 @@
       <c r="K71" s="47">
         <v>5</v>
       </c>
-      <c r="L71" s="185"/>
-      <c r="M71" s="178"/>
+      <c r="L71" s="183"/>
+      <c r="M71" s="176"/>
       <c r="N71" s="41"/>
       <c r="O71" s="38"/>
       <c r="P71" s="33"/>
@@ -5921,9 +5991,9 @@
       <c r="S71" s="15"/>
     </row>
     <row r="72" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="205"/>
-      <c r="B72" s="171"/>
-      <c r="C72" s="158"/>
+      <c r="A72" s="203"/>
+      <c r="B72" s="169"/>
+      <c r="C72" s="156"/>
       <c r="D72" s="39" t="s">
         <v>253</v>
       </c>
@@ -5945,11 +6015,11 @@
       <c r="J72" s="47">
         <v>5</v>
       </c>
-      <c r="K72" s="185">
-        <v>5</v>
-      </c>
-      <c r="L72" s="185"/>
-      <c r="M72" s="178"/>
+      <c r="K72" s="183">
+        <v>5</v>
+      </c>
+      <c r="L72" s="183"/>
+      <c r="M72" s="176"/>
       <c r="N72" s="41"/>
       <c r="O72" s="38"/>
       <c r="P72" s="33"/>
@@ -5958,9 +6028,9 @@
       <c r="S72" s="15"/>
     </row>
     <row r="73" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="205"/>
-      <c r="B73" s="171"/>
-      <c r="C73" s="158"/>
+      <c r="A73" s="203"/>
+      <c r="B73" s="169"/>
+      <c r="C73" s="156"/>
       <c r="D73" s="39" t="s">
         <v>253</v>
       </c>
@@ -5982,9 +6052,9 @@
       <c r="J73" s="47">
         <v>5</v>
       </c>
-      <c r="K73" s="185"/>
-      <c r="L73" s="185"/>
-      <c r="M73" s="178"/>
+      <c r="K73" s="183"/>
+      <c r="L73" s="183"/>
+      <c r="M73" s="176"/>
       <c r="N73" s="41"/>
       <c r="O73" s="38"/>
       <c r="P73" s="33"/>
@@ -5993,9 +6063,9 @@
       <c r="S73" s="15"/>
     </row>
     <row r="74" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="205"/>
-      <c r="B74" s="171"/>
-      <c r="C74" s="158"/>
+      <c r="A74" s="203"/>
+      <c r="B74" s="169"/>
+      <c r="C74" s="156"/>
       <c r="D74" s="39" t="s">
         <v>230</v>
       </c>
@@ -6020,8 +6090,8 @@
       <c r="K74" s="47">
         <v>5</v>
       </c>
-      <c r="L74" s="185"/>
-      <c r="M74" s="178"/>
+      <c r="L74" s="183"/>
+      <c r="M74" s="176"/>
       <c r="N74" s="41"/>
       <c r="O74" s="38"/>
       <c r="P74" s="33"/>
@@ -6030,9 +6100,9 @@
       <c r="S74" s="15"/>
     </row>
     <row r="75" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="205"/>
-      <c r="B75" s="171"/>
-      <c r="C75" s="158"/>
+      <c r="A75" s="203"/>
+      <c r="B75" s="169"/>
+      <c r="C75" s="156"/>
       <c r="D75" s="39" t="s">
         <v>232</v>
       </c>
@@ -6054,11 +6124,11 @@
       <c r="J75" s="47">
         <v>5</v>
       </c>
-      <c r="K75" s="185">
-        <v>5</v>
-      </c>
-      <c r="L75" s="185"/>
-      <c r="M75" s="178"/>
+      <c r="K75" s="183">
+        <v>5</v>
+      </c>
+      <c r="L75" s="183"/>
+      <c r="M75" s="176"/>
       <c r="N75" s="41"/>
       <c r="O75" s="38"/>
       <c r="P75" s="33"/>
@@ -6067,9 +6137,9 @@
       <c r="S75" s="15"/>
     </row>
     <row r="76" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="205"/>
-      <c r="B76" s="171"/>
-      <c r="C76" s="158"/>
+      <c r="A76" s="203"/>
+      <c r="B76" s="169"/>
+      <c r="C76" s="156"/>
       <c r="D76" s="39" t="s">
         <v>232</v>
       </c>
@@ -6091,9 +6161,9 @@
       <c r="J76" s="47">
         <v>5</v>
       </c>
-      <c r="K76" s="185"/>
-      <c r="L76" s="185"/>
-      <c r="M76" s="178"/>
+      <c r="K76" s="183"/>
+      <c r="L76" s="183"/>
+      <c r="M76" s="176"/>
       <c r="N76" s="41"/>
       <c r="O76" s="38"/>
       <c r="P76" s="33"/>
@@ -6102,9 +6172,9 @@
       <c r="S76" s="15"/>
     </row>
     <row r="77" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="205"/>
-      <c r="B77" s="171"/>
-      <c r="C77" s="158"/>
+      <c r="A77" s="203"/>
+      <c r="B77" s="169"/>
+      <c r="C77" s="156"/>
       <c r="D77" s="39" t="s">
         <v>235</v>
       </c>
@@ -6126,11 +6196,11 @@
       <c r="J77" s="47">
         <v>5</v>
       </c>
-      <c r="K77" s="185">
-        <v>5</v>
-      </c>
-      <c r="L77" s="185"/>
-      <c r="M77" s="178"/>
+      <c r="K77" s="183">
+        <v>5</v>
+      </c>
+      <c r="L77" s="183"/>
+      <c r="M77" s="176"/>
       <c r="N77" s="41"/>
       <c r="O77" s="38"/>
       <c r="P77" s="33"/>
@@ -6139,9 +6209,9 @@
       <c r="S77" s="15"/>
     </row>
     <row r="78" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="205"/>
-      <c r="B78" s="171"/>
-      <c r="C78" s="158"/>
+      <c r="A78" s="203"/>
+      <c r="B78" s="169"/>
+      <c r="C78" s="156"/>
       <c r="D78" s="39" t="s">
         <v>235</v>
       </c>
@@ -6163,9 +6233,9 @@
       <c r="J78" s="47">
         <v>5</v>
       </c>
-      <c r="K78" s="185"/>
-      <c r="L78" s="185"/>
-      <c r="M78" s="178"/>
+      <c r="K78" s="183"/>
+      <c r="L78" s="183"/>
+      <c r="M78" s="176"/>
       <c r="N78" s="41"/>
       <c r="O78" s="38"/>
       <c r="P78" s="33"/>
@@ -6174,9 +6244,9 @@
       <c r="S78" s="15"/>
     </row>
     <row r="79" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="205"/>
-      <c r="B79" s="171"/>
-      <c r="C79" s="158"/>
+      <c r="A79" s="203"/>
+      <c r="B79" s="169"/>
+      <c r="C79" s="156"/>
       <c r="D79" s="39" t="s">
         <v>235</v>
       </c>
@@ -6198,9 +6268,9 @@
       <c r="J79" s="47">
         <v>5</v>
       </c>
-      <c r="K79" s="185"/>
-      <c r="L79" s="185"/>
-      <c r="M79" s="178"/>
+      <c r="K79" s="183"/>
+      <c r="L79" s="183"/>
+      <c r="M79" s="176"/>
       <c r="N79" s="41"/>
       <c r="O79" s="38"/>
       <c r="P79" s="33"/>
@@ -6209,9 +6279,9 @@
       <c r="S79" s="15"/>
     </row>
     <row r="80" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="205"/>
-      <c r="B80" s="171"/>
-      <c r="C80" s="202" t="s">
+      <c r="A80" s="203"/>
+      <c r="B80" s="169"/>
+      <c r="C80" s="200" t="s">
         <v>24</v>
       </c>
       <c r="D80" s="39" t="s">
@@ -6238,10 +6308,10 @@
       <c r="K80" s="47">
         <v>5</v>
       </c>
-      <c r="L80" s="178">
-        <v>5</v>
-      </c>
-      <c r="M80" s="178"/>
+      <c r="L80" s="176">
+        <v>5</v>
+      </c>
+      <c r="M80" s="176"/>
       <c r="N80" s="41"/>
       <c r="O80" s="41"/>
       <c r="P80" s="49"/>
@@ -6250,9 +6320,9 @@
       <c r="S80" s="15"/>
     </row>
     <row r="81" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="205"/>
-      <c r="B81" s="171"/>
-      <c r="C81" s="202"/>
+      <c r="A81" s="203"/>
+      <c r="B81" s="169"/>
+      <c r="C81" s="200"/>
       <c r="D81" s="39" t="s">
         <v>228</v>
       </c>
@@ -6277,8 +6347,8 @@
       <c r="K81" s="47">
         <v>5</v>
       </c>
-      <c r="L81" s="178"/>
-      <c r="M81" s="178"/>
+      <c r="L81" s="176"/>
+      <c r="M81" s="176"/>
       <c r="N81" s="35"/>
       <c r="O81" s="35"/>
       <c r="P81" s="37"/>
@@ -6288,9 +6358,9 @@
       <c r="T81" s="6"/>
     </row>
     <row r="82" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="205"/>
-      <c r="B82" s="171"/>
-      <c r="C82" s="202"/>
+      <c r="A82" s="203"/>
+      <c r="B82" s="169"/>
+      <c r="C82" s="200"/>
       <c r="D82" s="39" t="s">
         <v>243</v>
       </c>
@@ -6315,8 +6385,8 @@
       <c r="K82" s="47">
         <v>5</v>
       </c>
-      <c r="L82" s="178"/>
-      <c r="M82" s="178"/>
+      <c r="L82" s="176"/>
+      <c r="M82" s="176"/>
       <c r="N82" s="35"/>
       <c r="O82" s="35"/>
       <c r="P82" s="37"/>
@@ -6326,9 +6396,9 @@
       <c r="T82" s="6"/>
     </row>
     <row r="83" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="205"/>
-      <c r="B83" s="171"/>
-      <c r="C83" s="202"/>
+      <c r="A83" s="203"/>
+      <c r="B83" s="169"/>
+      <c r="C83" s="200"/>
       <c r="D83" s="39" t="s">
         <v>74</v>
       </c>
@@ -6353,8 +6423,8 @@
       <c r="K83" s="47">
         <v>5</v>
       </c>
-      <c r="L83" s="178"/>
-      <c r="M83" s="178"/>
+      <c r="L83" s="176"/>
+      <c r="M83" s="176"/>
       <c r="N83" s="35"/>
       <c r="O83" s="35"/>
       <c r="P83" s="37"/>
@@ -6364,8 +6434,8 @@
       <c r="T83" s="6"/>
     </row>
     <row r="84" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="205"/>
-      <c r="B84" s="171" t="s">
+      <c r="A84" s="203"/>
+      <c r="B84" s="169" t="s">
         <v>25</v>
       </c>
       <c r="C84" s="39" t="s">
@@ -6398,7 +6468,7 @@
       <c r="L84" s="36">
         <v>5</v>
       </c>
-      <c r="M84" s="180">
+      <c r="M84" s="178">
         <v>7</v>
       </c>
       <c r="N84" s="35"/>
@@ -6414,8 +6484,8 @@
       <c r="T84" s="6"/>
     </row>
     <row r="85" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="205"/>
-      <c r="B85" s="171"/>
+      <c r="A85" s="203"/>
+      <c r="B85" s="169"/>
       <c r="C85" s="39" t="s">
         <v>27</v>
       </c>
@@ -6446,7 +6516,7 @@
       <c r="L85" s="36">
         <v>5</v>
       </c>
-      <c r="M85" s="180"/>
+      <c r="M85" s="178"/>
       <c r="N85" s="50"/>
       <c r="O85" s="35" t="s">
         <v>100</v>
@@ -6462,12 +6532,12 @@
       <c r="T85" s="6"/>
     </row>
     <row r="86" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="205"/>
-      <c r="B86" s="171"/>
-      <c r="C86" s="202" t="s">
+      <c r="A86" s="203"/>
+      <c r="B86" s="169"/>
+      <c r="C86" s="200" t="s">
         <v>28</v>
       </c>
-      <c r="D86" s="158" t="s">
+      <c r="D86" s="156" t="s">
         <v>97</v>
       </c>
       <c r="E86" s="32" t="s">
@@ -6488,13 +6558,13 @@
       <c r="J86" s="36">
         <v>5</v>
       </c>
-      <c r="K86" s="180">
+      <c r="K86" s="178">
         <v>8</v>
       </c>
-      <c r="L86" s="180">
+      <c r="L86" s="178">
         <v>9</v>
       </c>
-      <c r="M86" s="180"/>
+      <c r="M86" s="178"/>
       <c r="N86" s="35"/>
       <c r="O86" s="35" t="s">
         <v>29</v>
@@ -6508,10 +6578,10 @@
       <c r="T86" s="6"/>
     </row>
     <row r="87" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="205"/>
-      <c r="B87" s="171"/>
-      <c r="C87" s="202"/>
-      <c r="D87" s="158"/>
+      <c r="A87" s="203"/>
+      <c r="B87" s="169"/>
+      <c r="C87" s="200"/>
+      <c r="D87" s="156"/>
       <c r="E87" s="32" t="s">
         <v>141</v>
       </c>
@@ -6530,9 +6600,9 @@
       <c r="J87" s="36">
         <v>5</v>
       </c>
-      <c r="K87" s="180"/>
-      <c r="L87" s="180"/>
-      <c r="M87" s="180"/>
+      <c r="K87" s="178"/>
+      <c r="L87" s="178"/>
+      <c r="M87" s="178"/>
       <c r="N87" s="35"/>
       <c r="O87" s="35"/>
       <c r="P87" s="37"/>
@@ -6542,10 +6612,10 @@
       <c r="T87" s="6"/>
     </row>
     <row r="88" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="205"/>
-      <c r="B88" s="171"/>
-      <c r="C88" s="202"/>
-      <c r="D88" s="158"/>
+      <c r="A88" s="203"/>
+      <c r="B88" s="169"/>
+      <c r="C88" s="200"/>
+      <c r="D88" s="156"/>
       <c r="E88" s="32" t="s">
         <v>140</v>
       </c>
@@ -6564,9 +6634,9 @@
       <c r="J88" s="36">
         <v>5</v>
       </c>
-      <c r="K88" s="180"/>
-      <c r="L88" s="180"/>
-      <c r="M88" s="180"/>
+      <c r="K88" s="178"/>
+      <c r="L88" s="178"/>
+      <c r="M88" s="178"/>
       <c r="N88" s="35"/>
       <c r="O88" s="35"/>
       <c r="P88" s="37"/>
@@ -6576,16 +6646,16 @@
       <c r="T88" s="6"/>
     </row>
     <row r="89" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="205"/>
-      <c r="B89" s="171"/>
-      <c r="C89" s="202"/>
-      <c r="D89" s="158" t="s">
+      <c r="A89" s="203"/>
+      <c r="B89" s="169"/>
+      <c r="C89" s="200"/>
+      <c r="D89" s="156" t="s">
         <v>30</v>
       </c>
       <c r="E89" s="76" t="s">
         <v>102</v>
       </c>
-      <c r="F89" s="140" t="s">
+      <c r="F89" s="139" t="s">
         <v>143</v>
       </c>
       <c r="G89" s="76" t="s">
@@ -6600,11 +6670,11 @@
       <c r="J89" s="77">
         <v>7</v>
       </c>
-      <c r="K89" s="181">
+      <c r="K89" s="179">
         <v>7</v>
       </c>
-      <c r="L89" s="180"/>
-      <c r="M89" s="180"/>
+      <c r="L89" s="178"/>
+      <c r="M89" s="178"/>
       <c r="N89" s="78" t="s">
         <v>282</v>
       </c>
@@ -6620,10 +6690,10 @@
       <c r="T89" s="83"/>
     </row>
     <row r="90" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="205"/>
-      <c r="B90" s="171"/>
-      <c r="C90" s="202"/>
-      <c r="D90" s="158"/>
+      <c r="A90" s="203"/>
+      <c r="B90" s="169"/>
+      <c r="C90" s="200"/>
+      <c r="D90" s="156"/>
       <c r="E90" s="32" t="s">
         <v>147</v>
       </c>
@@ -6642,9 +6712,9 @@
       <c r="J90" s="36">
         <v>9</v>
       </c>
-      <c r="K90" s="181"/>
-      <c r="L90" s="180"/>
-      <c r="M90" s="180"/>
+      <c r="K90" s="179"/>
+      <c r="L90" s="178"/>
+      <c r="M90" s="178"/>
       <c r="N90" s="50"/>
       <c r="O90" s="45"/>
       <c r="P90" s="48" t="s">
@@ -6656,11 +6726,11 @@
       <c r="T90" s="6"/>
     </row>
     <row r="91" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="205"/>
-      <c r="B91" s="171" t="s">
+      <c r="A91" s="203"/>
+      <c r="B91" s="169" t="s">
         <v>31</v>
       </c>
-      <c r="C91" s="158" t="s">
+      <c r="C91" s="156" t="s">
         <v>32</v>
       </c>
       <c r="D91" s="39" t="s">
@@ -6687,10 +6757,10 @@
       <c r="K91" s="53">
         <v>8</v>
       </c>
-      <c r="L91" s="178">
+      <c r="L91" s="176">
         <v>8</v>
       </c>
-      <c r="M91" s="178">
+      <c r="M91" s="176">
         <v>8</v>
       </c>
       <c r="N91" s="41"/>
@@ -6703,9 +6773,9 @@
       <c r="S91" s="15"/>
     </row>
     <row r="92" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="205"/>
-      <c r="B92" s="171"/>
-      <c r="C92" s="158"/>
+      <c r="A92" s="203"/>
+      <c r="B92" s="169"/>
+      <c r="C92" s="156"/>
       <c r="D92" s="39" t="s">
         <v>179</v>
       </c>
@@ -6730,8 +6800,8 @@
       <c r="K92" s="53">
         <v>10</v>
       </c>
-      <c r="L92" s="178"/>
-      <c r="M92" s="178"/>
+      <c r="L92" s="176"/>
+      <c r="M92" s="176"/>
       <c r="N92" s="41" t="s">
         <v>113</v>
       </c>
@@ -6744,9 +6814,9 @@
       <c r="S92" s="15"/>
     </row>
     <row r="93" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="205"/>
-      <c r="B93" s="171"/>
-      <c r="C93" s="158" t="s">
+      <c r="A93" s="203"/>
+      <c r="B93" s="169"/>
+      <c r="C93" s="156" t="s">
         <v>33</v>
       </c>
       <c r="D93" s="39" t="s">
@@ -6773,13 +6843,13 @@
       <c r="K93" s="53">
         <v>5</v>
       </c>
-      <c r="L93" s="178">
+      <c r="L93" s="176">
         <v>8</v>
       </c>
-      <c r="M93" s="178"/>
+      <c r="M93" s="176"/>
       <c r="N93" s="41"/>
       <c r="O93" s="41"/>
-      <c r="P93" s="176" t="s">
+      <c r="P93" s="174" t="s">
         <v>94</v>
       </c>
       <c r="Q93" s="41" t="s">
@@ -6789,9 +6859,9 @@
       <c r="S93" s="15"/>
     </row>
     <row r="94" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="205"/>
-      <c r="B94" s="171"/>
-      <c r="C94" s="158"/>
+      <c r="A94" s="203"/>
+      <c r="B94" s="169"/>
+      <c r="C94" s="156"/>
       <c r="D94" s="39" t="s">
         <v>106</v>
       </c>
@@ -6816,11 +6886,11 @@
       <c r="K94" s="53">
         <v>5</v>
       </c>
-      <c r="L94" s="178"/>
-      <c r="M94" s="178"/>
+      <c r="L94" s="176"/>
+      <c r="M94" s="176"/>
       <c r="N94" s="41"/>
       <c r="O94" s="41"/>
-      <c r="P94" s="176"/>
+      <c r="P94" s="174"/>
       <c r="Q94" s="41" t="s">
         <v>104</v>
       </c>
@@ -6828,9 +6898,9 @@
       <c r="S94" s="15"/>
     </row>
     <row r="95" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="205"/>
-      <c r="B95" s="171"/>
-      <c r="C95" s="158" t="s">
+      <c r="A95" s="203"/>
+      <c r="B95" s="169"/>
+      <c r="C95" s="156" t="s">
         <v>34</v>
       </c>
       <c r="D95" s="39" t="s">
@@ -6857,15 +6927,15 @@
       <c r="K95" s="53">
         <v>5</v>
       </c>
-      <c r="L95" s="178">
-        <v>5</v>
-      </c>
-      <c r="M95" s="178"/>
+      <c r="L95" s="176">
+        <v>5</v>
+      </c>
+      <c r="M95" s="176"/>
       <c r="N95" s="41" t="s">
         <v>114</v>
       </c>
       <c r="O95" s="41"/>
-      <c r="P95" s="176"/>
+      <c r="P95" s="174"/>
       <c r="Q95" s="41" t="s">
         <v>112</v>
       </c>
@@ -6873,9 +6943,9 @@
       <c r="S95" s="15"/>
     </row>
     <row r="96" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="205"/>
-      <c r="B96" s="171"/>
-      <c r="C96" s="158"/>
+      <c r="A96" s="203"/>
+      <c r="B96" s="169"/>
+      <c r="C96" s="156"/>
       <c r="D96" s="39" t="s">
         <v>108</v>
       </c>
@@ -6900,11 +6970,11 @@
       <c r="K96" s="53">
         <v>10</v>
       </c>
-      <c r="L96" s="178"/>
-      <c r="M96" s="178"/>
+      <c r="L96" s="176"/>
+      <c r="M96" s="176"/>
       <c r="N96" s="41"/>
       <c r="O96" s="41"/>
-      <c r="P96" s="176"/>
+      <c r="P96" s="174"/>
       <c r="Q96" s="41" t="s">
         <v>109</v>
       </c>
@@ -6912,9 +6982,9 @@
       <c r="S96" s="15"/>
     </row>
     <row r="97" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="205"/>
-      <c r="B97" s="171"/>
-      <c r="C97" s="158" t="s">
+      <c r="A97" s="203"/>
+      <c r="B97" s="169"/>
+      <c r="C97" s="156" t="s">
         <v>172</v>
       </c>
       <c r="D97" s="39" t="s">
@@ -6941,13 +7011,13 @@
       <c r="K97" s="53">
         <v>6</v>
       </c>
-      <c r="L97" s="178" t="s">
+      <c r="L97" s="176" t="s">
         <v>265</v>
       </c>
-      <c r="M97" s="178"/>
+      <c r="M97" s="176"/>
       <c r="N97" s="41"/>
       <c r="O97" s="41"/>
-      <c r="P97" s="176"/>
+      <c r="P97" s="174"/>
       <c r="Q97" s="41" t="s">
         <v>264</v>
       </c>
@@ -6955,9 +7025,9 @@
       <c r="S97" s="15"/>
     </row>
     <row r="98" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="206"/>
-      <c r="B98" s="190"/>
-      <c r="C98" s="162"/>
+      <c r="A98" s="204"/>
+      <c r="B98" s="188"/>
+      <c r="C98" s="160"/>
       <c r="D98" s="95" t="s">
         <v>174</v>
       </c>
@@ -6982,11 +7052,11 @@
       <c r="K98" s="99">
         <v>4</v>
       </c>
-      <c r="L98" s="179"/>
-      <c r="M98" s="179"/>
+      <c r="L98" s="177"/>
+      <c r="M98" s="177"/>
       <c r="N98" s="98"/>
       <c r="O98" s="98"/>
-      <c r="P98" s="177"/>
+      <c r="P98" s="175"/>
       <c r="Q98" s="98" t="s">
         <v>264</v>
       </c>
@@ -6994,7 +7064,7 @@
       <c r="S98" s="15"/>
     </row>
     <row r="99" spans="1:19" s="12" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="199" t="s">
+      <c r="A99" s="197" t="s">
         <v>35</v>
       </c>
       <c r="B99" s="131"/>
@@ -7017,308 +7087,310 @@
       <c r="S99" s="28"/>
     </row>
     <row r="100" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="200"/>
-      <c r="B100" s="164" t="s">
+      <c r="A100" s="198"/>
+      <c r="B100" s="162" t="s">
         <v>316</v>
       </c>
-      <c r="C100" s="226" t="s">
+      <c r="C100" s="224" t="s">
         <v>317</v>
       </c>
-      <c r="D100" s="226" t="s">
+      <c r="D100" s="224" t="s">
         <v>317</v>
       </c>
-      <c r="E100" s="226" t="s">
+      <c r="E100" s="224" t="s">
         <v>317</v>
       </c>
-      <c r="F100" s="227" t="s">
+      <c r="F100" s="225" t="s">
         <v>143</v>
       </c>
-      <c r="G100" s="228" t="s">
+      <c r="G100" s="226" t="s">
         <v>198</v>
       </c>
       <c r="H100" s="130" t="s">
         <v>337</v>
       </c>
-      <c r="I100" s="114"/>
-      <c r="J100" s="138"/>
-      <c r="K100" s="138"/>
-      <c r="L100" s="138"/>
-      <c r="M100" s="138"/>
+      <c r="I100" s="234" t="s">
+        <v>198</v>
+      </c>
+      <c r="J100" s="235"/>
+      <c r="K100" s="235"/>
+      <c r="L100" s="235"/>
+      <c r="M100" s="236"/>
       <c r="N100" s="114"/>
       <c r="O100" s="114"/>
       <c r="P100" s="116"/>
       <c r="Q100" s="114"/>
-      <c r="R100" s="139"/>
+      <c r="R100" s="138"/>
       <c r="S100" s="15"/>
     </row>
     <row r="101" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="200"/>
-      <c r="B101" s="165"/>
-      <c r="C101" s="158" t="s">
+      <c r="A101" s="198"/>
+      <c r="B101" s="163"/>
+      <c r="C101" s="156" t="s">
         <v>313</v>
       </c>
-      <c r="D101" s="158" t="s">
+      <c r="D101" s="156" t="s">
         <v>77</v>
       </c>
-      <c r="E101" s="152" t="s">
+      <c r="E101" s="150" t="s">
         <v>78</v>
       </c>
-      <c r="F101" s="155" t="s">
+      <c r="F101" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G101" s="155" t="s">
+      <c r="G101" s="153" t="s">
         <v>198</v>
       </c>
       <c r="H101" s="130" t="s">
         <v>337</v>
       </c>
-      <c r="I101" s="130"/>
-      <c r="J101" s="148"/>
-      <c r="K101" s="148"/>
-      <c r="L101" s="148"/>
-      <c r="M101" s="148"/>
+      <c r="I101" s="237"/>
+      <c r="J101" s="238"/>
+      <c r="K101" s="238"/>
+      <c r="L101" s="238"/>
+      <c r="M101" s="239"/>
       <c r="N101" s="130"/>
       <c r="O101" s="130"/>
-      <c r="P101" s="147"/>
+      <c r="P101" s="146"/>
       <c r="Q101" s="130"/>
-      <c r="R101" s="149"/>
+      <c r="R101" s="147"/>
       <c r="S101" s="15"/>
     </row>
     <row r="102" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="200"/>
-      <c r="B102" s="166"/>
-      <c r="C102" s="158"/>
-      <c r="D102" s="158"/>
-      <c r="E102" s="152" t="s">
+      <c r="A102" s="198"/>
+      <c r="B102" s="164"/>
+      <c r="C102" s="156"/>
+      <c r="D102" s="156"/>
+      <c r="E102" s="150" t="s">
         <v>80</v>
       </c>
-      <c r="F102" s="155" t="s">
+      <c r="F102" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G102" s="155" t="s">
+      <c r="G102" s="153" t="s">
         <v>198</v>
       </c>
       <c r="H102" s="130" t="s">
         <v>337</v>
       </c>
-      <c r="I102" s="130"/>
-      <c r="J102" s="148"/>
-      <c r="K102" s="148"/>
-      <c r="L102" s="148"/>
-      <c r="M102" s="148"/>
+      <c r="I102" s="237"/>
+      <c r="J102" s="238"/>
+      <c r="K102" s="238"/>
+      <c r="L102" s="238"/>
+      <c r="M102" s="239"/>
       <c r="N102" s="130"/>
       <c r="O102" s="130"/>
-      <c r="P102" s="147"/>
+      <c r="P102" s="146"/>
       <c r="Q102" s="130"/>
-      <c r="R102" s="149"/>
+      <c r="R102" s="147"/>
       <c r="S102" s="15"/>
     </row>
     <row r="103" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="200"/>
-      <c r="B103" s="166"/>
-      <c r="C103" s="158"/>
-      <c r="D103" s="152" t="s">
+      <c r="A103" s="198"/>
+      <c r="B103" s="164"/>
+      <c r="C103" s="156"/>
+      <c r="D103" s="150" t="s">
         <v>81</v>
       </c>
-      <c r="E103" s="152" t="s">
+      <c r="E103" s="150" t="s">
         <v>82</v>
       </c>
-      <c r="F103" s="155" t="s">
+      <c r="F103" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G103" s="155" t="s">
+      <c r="G103" s="153" t="s">
         <v>198</v>
       </c>
       <c r="H103" s="130" t="s">
         <v>337</v>
       </c>
-      <c r="I103" s="130"/>
-      <c r="J103" s="148"/>
-      <c r="K103" s="148"/>
-      <c r="L103" s="148"/>
-      <c r="M103" s="148"/>
+      <c r="I103" s="237"/>
+      <c r="J103" s="238"/>
+      <c r="K103" s="238"/>
+      <c r="L103" s="238"/>
+      <c r="M103" s="239"/>
       <c r="N103" s="130"/>
       <c r="O103" s="130"/>
-      <c r="P103" s="147"/>
+      <c r="P103" s="146"/>
       <c r="Q103" s="130"/>
-      <c r="R103" s="149"/>
+      <c r="R103" s="147"/>
       <c r="S103" s="15"/>
     </row>
     <row r="104" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="200"/>
-      <c r="B104" s="166"/>
-      <c r="C104" s="158"/>
-      <c r="D104" s="158" t="s">
+      <c r="A104" s="198"/>
+      <c r="B104" s="164"/>
+      <c r="C104" s="156"/>
+      <c r="D104" s="156" t="s">
         <v>83</v>
       </c>
-      <c r="E104" s="152" t="s">
+      <c r="E104" s="150" t="s">
         <v>84</v>
       </c>
-      <c r="F104" s="155" t="s">
+      <c r="F104" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G104" s="155" t="s">
+      <c r="G104" s="153" t="s">
         <v>198</v>
       </c>
       <c r="H104" s="130" t="s">
         <v>337</v>
       </c>
-      <c r="I104" s="130"/>
-      <c r="J104" s="148"/>
-      <c r="K104" s="148"/>
-      <c r="L104" s="148"/>
-      <c r="M104" s="148"/>
+      <c r="I104" s="237"/>
+      <c r="J104" s="238"/>
+      <c r="K104" s="238"/>
+      <c r="L104" s="238"/>
+      <c r="M104" s="239"/>
       <c r="N104" s="130"/>
       <c r="O104" s="130"/>
-      <c r="P104" s="147"/>
+      <c r="P104" s="146"/>
       <c r="Q104" s="130"/>
-      <c r="R104" s="149"/>
+      <c r="R104" s="147"/>
       <c r="S104" s="15"/>
     </row>
     <row r="105" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="200"/>
-      <c r="B105" s="166"/>
-      <c r="C105" s="158"/>
-      <c r="D105" s="158"/>
-      <c r="E105" s="152" t="s">
+      <c r="A105" s="198"/>
+      <c r="B105" s="164"/>
+      <c r="C105" s="156"/>
+      <c r="D105" s="156"/>
+      <c r="E105" s="150" t="s">
         <v>85</v>
       </c>
-      <c r="F105" s="155" t="s">
+      <c r="F105" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G105" s="155" t="s">
+      <c r="G105" s="153" t="s">
         <v>198</v>
       </c>
       <c r="H105" s="130" t="s">
         <v>337</v>
       </c>
-      <c r="I105" s="130"/>
-      <c r="J105" s="148"/>
-      <c r="K105" s="148"/>
-      <c r="L105" s="148"/>
-      <c r="M105" s="148"/>
+      <c r="I105" s="237"/>
+      <c r="J105" s="238"/>
+      <c r="K105" s="238"/>
+      <c r="L105" s="238"/>
+      <c r="M105" s="239"/>
       <c r="N105" s="130"/>
       <c r="O105" s="130"/>
-      <c r="P105" s="147"/>
+      <c r="P105" s="146"/>
       <c r="Q105" s="130"/>
-      <c r="R105" s="149"/>
+      <c r="R105" s="147"/>
       <c r="S105" s="15"/>
     </row>
     <row r="106" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="200"/>
-      <c r="B106" s="166"/>
-      <c r="C106" s="158"/>
-      <c r="D106" s="158"/>
-      <c r="E106" s="152" t="s">
+      <c r="A106" s="198"/>
+      <c r="B106" s="164"/>
+      <c r="C106" s="156"/>
+      <c r="D106" s="156"/>
+      <c r="E106" s="150" t="s">
         <v>86</v>
       </c>
-      <c r="F106" s="155" t="s">
+      <c r="F106" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G106" s="155" t="s">
+      <c r="G106" s="153" t="s">
         <v>198</v>
       </c>
       <c r="H106" s="130" t="s">
         <v>337</v>
       </c>
-      <c r="I106" s="130"/>
-      <c r="J106" s="148"/>
-      <c r="K106" s="148"/>
-      <c r="L106" s="148"/>
-      <c r="M106" s="148"/>
+      <c r="I106" s="237"/>
+      <c r="J106" s="238"/>
+      <c r="K106" s="238"/>
+      <c r="L106" s="238"/>
+      <c r="M106" s="239"/>
       <c r="N106" s="130"/>
       <c r="O106" s="130"/>
-      <c r="P106" s="147"/>
+      <c r="P106" s="146"/>
       <c r="Q106" s="130"/>
-      <c r="R106" s="149"/>
+      <c r="R106" s="147"/>
       <c r="S106" s="15"/>
     </row>
     <row r="107" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="200"/>
-      <c r="B107" s="166"/>
-      <c r="C107" s="158" t="s">
+      <c r="A107" s="198"/>
+      <c r="B107" s="164"/>
+      <c r="C107" s="156" t="s">
         <v>314</v>
       </c>
-      <c r="D107" s="158" t="s">
+      <c r="D107" s="156" t="s">
         <v>77</v>
       </c>
-      <c r="E107" s="152" t="s">
+      <c r="E107" s="150" t="s">
         <v>78</v>
       </c>
-      <c r="F107" s="155" t="s">
+      <c r="F107" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G107" s="155" t="s">
+      <c r="G107" s="153" t="s">
         <v>198</v>
       </c>
       <c r="H107" s="130" t="s">
         <v>337</v>
       </c>
-      <c r="I107" s="130"/>
-      <c r="J107" s="148"/>
-      <c r="K107" s="148"/>
-      <c r="L107" s="148"/>
-      <c r="M107" s="148"/>
+      <c r="I107" s="237"/>
+      <c r="J107" s="238"/>
+      <c r="K107" s="238"/>
+      <c r="L107" s="238"/>
+      <c r="M107" s="239"/>
       <c r="N107" s="130"/>
       <c r="O107" s="130"/>
-      <c r="P107" s="147"/>
+      <c r="P107" s="146"/>
       <c r="Q107" s="130"/>
-      <c r="R107" s="149"/>
+      <c r="R107" s="147"/>
       <c r="S107" s="15"/>
     </row>
     <row r="108" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="200"/>
-      <c r="B108" s="166"/>
-      <c r="C108" s="158"/>
-      <c r="D108" s="158"/>
-      <c r="E108" s="152" t="s">
+      <c r="A108" s="198"/>
+      <c r="B108" s="164"/>
+      <c r="C108" s="156"/>
+      <c r="D108" s="156"/>
+      <c r="E108" s="150" t="s">
         <v>80</v>
       </c>
-      <c r="F108" s="155" t="s">
+      <c r="F108" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G108" s="155" t="s">
+      <c r="G108" s="153" t="s">
         <v>198</v>
       </c>
       <c r="H108" s="130" t="s">
         <v>337</v>
       </c>
-      <c r="I108" s="130"/>
-      <c r="J108" s="148"/>
-      <c r="K108" s="148"/>
-      <c r="L108" s="148"/>
-      <c r="M108" s="148"/>
+      <c r="I108" s="237"/>
+      <c r="J108" s="238"/>
+      <c r="K108" s="238"/>
+      <c r="L108" s="238"/>
+      <c r="M108" s="239"/>
       <c r="N108" s="130"/>
       <c r="O108" s="130"/>
-      <c r="P108" s="147"/>
+      <c r="P108" s="146"/>
       <c r="Q108" s="130"/>
-      <c r="R108" s="149"/>
+      <c r="R108" s="147"/>
       <c r="S108" s="15"/>
     </row>
     <row r="109" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="200"/>
-      <c r="B109" s="166"/>
-      <c r="C109" s="158"/>
-      <c r="D109" s="152" t="s">
+      <c r="A109" s="198"/>
+      <c r="B109" s="164"/>
+      <c r="C109" s="156"/>
+      <c r="D109" s="150" t="s">
         <v>81</v>
       </c>
-      <c r="E109" s="152" t="s">
+      <c r="E109" s="150" t="s">
         <v>82</v>
       </c>
-      <c r="F109" s="155" t="s">
+      <c r="F109" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G109" s="155" t="s">
+      <c r="G109" s="153" t="s">
         <v>198</v>
       </c>
       <c r="H109" s="130" t="s">
         <v>337</v>
       </c>
-      <c r="I109" s="41"/>
-      <c r="J109" s="53"/>
-      <c r="K109" s="53"/>
-      <c r="L109" s="53"/>
-      <c r="M109" s="53"/>
+      <c r="I109" s="237"/>
+      <c r="J109" s="238"/>
+      <c r="K109" s="238"/>
+      <c r="L109" s="238"/>
+      <c r="M109" s="239"/>
       <c r="N109" s="41"/>
       <c r="O109" s="41"/>
       <c r="P109" s="49"/>
@@ -7327,29 +7399,29 @@
       <c r="S109" s="15"/>
     </row>
     <row r="110" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="200"/>
-      <c r="B110" s="166"/>
-      <c r="C110" s="158"/>
-      <c r="D110" s="158" t="s">
+      <c r="A110" s="198"/>
+      <c r="B110" s="164"/>
+      <c r="C110" s="156"/>
+      <c r="D110" s="156" t="s">
         <v>83</v>
       </c>
-      <c r="E110" s="152" t="s">
+      <c r="E110" s="150" t="s">
         <v>84</v>
       </c>
-      <c r="F110" s="155" t="s">
+      <c r="F110" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G110" s="155" t="s">
+      <c r="G110" s="153" t="s">
         <v>198</v>
       </c>
       <c r="H110" s="130" t="s">
         <v>337</v>
       </c>
-      <c r="I110" s="41"/>
-      <c r="J110" s="53"/>
-      <c r="K110" s="53"/>
-      <c r="L110" s="53"/>
-      <c r="M110" s="53"/>
+      <c r="I110" s="237"/>
+      <c r="J110" s="238"/>
+      <c r="K110" s="238"/>
+      <c r="L110" s="238"/>
+      <c r="M110" s="239"/>
       <c r="N110" s="41"/>
       <c r="O110" s="41"/>
       <c r="P110" s="49"/>
@@ -7358,27 +7430,27 @@
       <c r="S110" s="15"/>
     </row>
     <row r="111" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="200"/>
-      <c r="B111" s="166"/>
-      <c r="C111" s="158"/>
-      <c r="D111" s="158"/>
-      <c r="E111" s="152" t="s">
+      <c r="A111" s="198"/>
+      <c r="B111" s="164"/>
+      <c r="C111" s="156"/>
+      <c r="D111" s="156"/>
+      <c r="E111" s="150" t="s">
         <v>85</v>
       </c>
-      <c r="F111" s="155" t="s">
+      <c r="F111" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G111" s="155" t="s">
+      <c r="G111" s="153" t="s">
         <v>198</v>
       </c>
       <c r="H111" s="130" t="s">
         <v>337</v>
       </c>
-      <c r="I111" s="41"/>
-      <c r="J111" s="53"/>
-      <c r="K111" s="53"/>
-      <c r="L111" s="53"/>
-      <c r="M111" s="53"/>
+      <c r="I111" s="237"/>
+      <c r="J111" s="238"/>
+      <c r="K111" s="238"/>
+      <c r="L111" s="238"/>
+      <c r="M111" s="239"/>
       <c r="N111" s="41"/>
       <c r="O111" s="35"/>
       <c r="P111" s="37"/>
@@ -7387,27 +7459,27 @@
       <c r="S111" s="26"/>
     </row>
     <row r="112" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="200"/>
-      <c r="B112" s="166"/>
-      <c r="C112" s="158"/>
-      <c r="D112" s="158"/>
-      <c r="E112" s="152" t="s">
+      <c r="A112" s="198"/>
+      <c r="B112" s="164"/>
+      <c r="C112" s="156"/>
+      <c r="D112" s="156"/>
+      <c r="E112" s="150" t="s">
         <v>86</v>
       </c>
-      <c r="F112" s="155" t="s">
+      <c r="F112" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G112" s="155" t="s">
+      <c r="G112" s="153" t="s">
         <v>198</v>
       </c>
       <c r="H112" s="130" t="s">
         <v>337</v>
       </c>
-      <c r="I112" s="41"/>
-      <c r="J112" s="53"/>
-      <c r="K112" s="53"/>
-      <c r="L112" s="53"/>
-      <c r="M112" s="53"/>
+      <c r="I112" s="237"/>
+      <c r="J112" s="238"/>
+      <c r="K112" s="238"/>
+      <c r="L112" s="238"/>
+      <c r="M112" s="239"/>
       <c r="N112" s="41"/>
       <c r="O112" s="35"/>
       <c r="P112" s="37"/>
@@ -7416,31 +7488,31 @@
       <c r="S112" s="26"/>
     </row>
     <row r="113" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="200"/>
-      <c r="B113" s="166"/>
-      <c r="C113" s="158" t="s">
+      <c r="A113" s="198"/>
+      <c r="B113" s="164"/>
+      <c r="C113" s="156" t="s">
         <v>315</v>
       </c>
-      <c r="D113" s="158" t="s">
+      <c r="D113" s="156" t="s">
         <v>77</v>
       </c>
-      <c r="E113" s="152" t="s">
+      <c r="E113" s="150" t="s">
         <v>78</v>
       </c>
-      <c r="F113" s="155" t="s">
+      <c r="F113" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G113" s="155" t="s">
+      <c r="G113" s="153" t="s">
         <v>198</v>
       </c>
       <c r="H113" s="130" t="s">
         <v>337</v>
       </c>
-      <c r="I113" s="41"/>
-      <c r="J113" s="53"/>
-      <c r="K113" s="53"/>
-      <c r="L113" s="53"/>
-      <c r="M113" s="53"/>
+      <c r="I113" s="237"/>
+      <c r="J113" s="238"/>
+      <c r="K113" s="238"/>
+      <c r="L113" s="238"/>
+      <c r="M113" s="239"/>
       <c r="N113" s="41"/>
       <c r="O113" s="35"/>
       <c r="P113" s="37"/>
@@ -7449,173 +7521,173 @@
       <c r="S113" s="26"/>
     </row>
     <row r="114" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="200"/>
-      <c r="B114" s="166"/>
-      <c r="C114" s="158"/>
-      <c r="D114" s="158"/>
-      <c r="E114" s="152" t="s">
+      <c r="A114" s="198"/>
+      <c r="B114" s="164"/>
+      <c r="C114" s="156"/>
+      <c r="D114" s="156"/>
+      <c r="E114" s="150" t="s">
         <v>80</v>
       </c>
-      <c r="F114" s="155" t="s">
+      <c r="F114" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G114" s="155" t="s">
+      <c r="G114" s="153" t="s">
         <v>198</v>
       </c>
       <c r="H114" s="130" t="s">
         <v>337</v>
       </c>
-      <c r="I114" s="145"/>
-      <c r="J114" s="53"/>
-      <c r="K114" s="99"/>
-      <c r="L114" s="53"/>
-      <c r="M114" s="53"/>
-      <c r="N114" s="145"/>
+      <c r="I114" s="237"/>
+      <c r="J114" s="238"/>
+      <c r="K114" s="238"/>
+      <c r="L114" s="238"/>
+      <c r="M114" s="239"/>
+      <c r="N114" s="144"/>
       <c r="O114" s="35"/>
-      <c r="P114" s="143"/>
+      <c r="P114" s="142"/>
       <c r="Q114" s="35"/>
       <c r="R114" s="61"/>
       <c r="S114" s="26"/>
     </row>
     <row r="115" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="200"/>
-      <c r="B115" s="166"/>
-      <c r="C115" s="158"/>
-      <c r="D115" s="152" t="s">
+      <c r="A115" s="198"/>
+      <c r="B115" s="164"/>
+      <c r="C115" s="156"/>
+      <c r="D115" s="150" t="s">
         <v>81</v>
       </c>
-      <c r="E115" s="152" t="s">
+      <c r="E115" s="150" t="s">
         <v>82</v>
       </c>
-      <c r="F115" s="155" t="s">
+      <c r="F115" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G115" s="155" t="s">
+      <c r="G115" s="153" t="s">
         <v>198</v>
       </c>
       <c r="H115" s="130" t="s">
         <v>337</v>
       </c>
-      <c r="I115" s="145"/>
-      <c r="J115" s="53"/>
-      <c r="K115" s="99"/>
-      <c r="L115" s="53"/>
-      <c r="M115" s="53"/>
-      <c r="N115" s="145"/>
+      <c r="I115" s="237"/>
+      <c r="J115" s="238"/>
+      <c r="K115" s="238"/>
+      <c r="L115" s="238"/>
+      <c r="M115" s="239"/>
+      <c r="N115" s="144"/>
       <c r="O115" s="35"/>
-      <c r="P115" s="143"/>
+      <c r="P115" s="142"/>
       <c r="Q115" s="35"/>
       <c r="R115" s="61"/>
       <c r="S115" s="26"/>
     </row>
     <row r="116" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="200"/>
-      <c r="B116" s="166"/>
-      <c r="C116" s="158"/>
-      <c r="D116" s="158" t="s">
+      <c r="A116" s="198"/>
+      <c r="B116" s="164"/>
+      <c r="C116" s="156"/>
+      <c r="D116" s="156" t="s">
         <v>83</v>
       </c>
-      <c r="E116" s="152" t="s">
+      <c r="E116" s="150" t="s">
         <v>84</v>
       </c>
-      <c r="F116" s="155" t="s">
+      <c r="F116" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G116" s="155" t="s">
+      <c r="G116" s="153" t="s">
         <v>198</v>
       </c>
       <c r="H116" s="130" t="s">
         <v>337</v>
       </c>
-      <c r="I116" s="145"/>
-      <c r="J116" s="53"/>
-      <c r="K116" s="99"/>
-      <c r="L116" s="53"/>
-      <c r="M116" s="53"/>
-      <c r="N116" s="145"/>
+      <c r="I116" s="237"/>
+      <c r="J116" s="238"/>
+      <c r="K116" s="238"/>
+      <c r="L116" s="238"/>
+      <c r="M116" s="239"/>
+      <c r="N116" s="144"/>
       <c r="O116" s="35"/>
-      <c r="P116" s="143"/>
+      <c r="P116" s="142"/>
       <c r="Q116" s="35"/>
       <c r="R116" s="61"/>
       <c r="S116" s="26"/>
     </row>
     <row r="117" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="200"/>
-      <c r="B117" s="166"/>
-      <c r="C117" s="158"/>
-      <c r="D117" s="158"/>
-      <c r="E117" s="152" t="s">
+      <c r="A117" s="198"/>
+      <c r="B117" s="164"/>
+      <c r="C117" s="156"/>
+      <c r="D117" s="156"/>
+      <c r="E117" s="150" t="s">
         <v>85</v>
       </c>
-      <c r="F117" s="155" t="s">
+      <c r="F117" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G117" s="155" t="s">
+      <c r="G117" s="153" t="s">
         <v>198</v>
       </c>
       <c r="H117" s="130" t="s">
         <v>337</v>
       </c>
-      <c r="I117" s="145"/>
-      <c r="J117" s="53"/>
-      <c r="K117" s="99"/>
-      <c r="L117" s="53"/>
-      <c r="M117" s="53"/>
-      <c r="N117" s="145"/>
+      <c r="I117" s="237"/>
+      <c r="J117" s="238"/>
+      <c r="K117" s="238"/>
+      <c r="L117" s="238"/>
+      <c r="M117" s="239"/>
+      <c r="N117" s="144"/>
       <c r="O117" s="35"/>
-      <c r="P117" s="143"/>
+      <c r="P117" s="142"/>
       <c r="Q117" s="35"/>
       <c r="R117" s="61"/>
       <c r="S117" s="26"/>
     </row>
     <row r="118" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="200"/>
-      <c r="B118" s="166"/>
-      <c r="C118" s="158"/>
-      <c r="D118" s="158"/>
-      <c r="E118" s="152" t="s">
+      <c r="A118" s="198"/>
+      <c r="B118" s="164"/>
+      <c r="C118" s="156"/>
+      <c r="D118" s="156"/>
+      <c r="E118" s="150" t="s">
         <v>86</v>
       </c>
-      <c r="F118" s="155" t="s">
+      <c r="F118" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G118" s="155" t="s">
+      <c r="G118" s="153" t="s">
         <v>198</v>
       </c>
       <c r="H118" s="130" t="s">
         <v>337</v>
       </c>
-      <c r="I118" s="145"/>
-      <c r="J118" s="53"/>
-      <c r="K118" s="99"/>
-      <c r="L118" s="53"/>
-      <c r="M118" s="53"/>
-      <c r="N118" s="145"/>
+      <c r="I118" s="240"/>
+      <c r="J118" s="241"/>
+      <c r="K118" s="241"/>
+      <c r="L118" s="241"/>
+      <c r="M118" s="242"/>
+      <c r="N118" s="144"/>
       <c r="O118" s="35"/>
-      <c r="P118" s="143"/>
+      <c r="P118" s="142"/>
       <c r="Q118" s="35"/>
       <c r="R118" s="61"/>
       <c r="S118" s="26"/>
     </row>
     <row r="119" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="200"/>
-      <c r="B119" s="166" t="s">
+      <c r="A119" s="198"/>
+      <c r="B119" s="164" t="s">
         <v>350</v>
       </c>
-      <c r="C119" s="229" t="s">
+      <c r="C119" s="227" t="s">
         <v>361</v>
       </c>
-      <c r="D119" s="224" t="s">
+      <c r="D119" s="222" t="s">
         <v>348</v>
       </c>
-      <c r="E119" s="224" t="s">
+      <c r="E119" s="222" t="s">
         <v>348</v>
       </c>
-      <c r="F119" s="155" t="s">
+      <c r="F119" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G119" s="153"/>
-      <c r="H119" s="145"/>
+      <c r="G119" s="151"/>
+      <c r="H119" s="144"/>
       <c r="I119" s="35"/>
       <c r="J119" s="36">
         <v>5</v>
@@ -7623,172 +7695,172 @@
       <c r="K119" s="36">
         <v>10</v>
       </c>
-      <c r="L119" s="159">
+      <c r="L119" s="157">
         <v>8</v>
       </c>
-      <c r="M119" s="159">
+      <c r="M119" s="157">
         <v>7</v>
       </c>
       <c r="N119" s="35"/>
-      <c r="O119" s="145"/>
-      <c r="P119" s="141"/>
+      <c r="O119" s="144"/>
+      <c r="P119" s="140"/>
       <c r="Q119" s="35"/>
       <c r="R119" s="63"/>
       <c r="S119" s="26"/>
     </row>
     <row r="120" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="200"/>
-      <c r="B120" s="166"/>
-      <c r="C120" s="229"/>
-      <c r="D120" s="224" t="s">
+      <c r="A120" s="198"/>
+      <c r="B120" s="164"/>
+      <c r="C120" s="227"/>
+      <c r="D120" s="222" t="s">
         <v>349</v>
       </c>
-      <c r="E120" s="224" t="s">
+      <c r="E120" s="222" t="s">
         <v>349</v>
       </c>
-      <c r="F120" s="155" t="s">
+      <c r="F120" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G120" s="153"/>
-      <c r="H120" s="145"/>
+      <c r="G120" s="151"/>
+      <c r="H120" s="144"/>
       <c r="I120" s="35"/>
       <c r="J120" s="36">
         <v>5</v>
       </c>
-      <c r="K120" s="214">
-        <v>5</v>
-      </c>
-      <c r="L120" s="160"/>
-      <c r="M120" s="160"/>
+      <c r="K120" s="212">
+        <v>5</v>
+      </c>
+      <c r="L120" s="158"/>
+      <c r="M120" s="158"/>
       <c r="N120" s="35"/>
-      <c r="O120" s="145"/>
-      <c r="P120" s="141"/>
+      <c r="O120" s="144"/>
+      <c r="P120" s="140"/>
       <c r="Q120" s="35"/>
       <c r="R120" s="63"/>
       <c r="S120" s="26"/>
     </row>
     <row r="121" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="200"/>
-      <c r="B121" s="166"/>
-      <c r="C121" s="229"/>
-      <c r="D121" s="230" t="s">
+      <c r="A121" s="198"/>
+      <c r="B121" s="164"/>
+      <c r="C121" s="227"/>
+      <c r="D121" s="228" t="s">
         <v>362</v>
       </c>
-      <c r="E121" s="152" t="s">
+      <c r="E121" s="150" t="s">
         <v>363</v>
       </c>
-      <c r="F121" s="155" t="s">
+      <c r="F121" s="153" t="s">
         <v>143</v>
       </c>
       <c r="G121" s="35" t="s">
         <v>368</v>
       </c>
-      <c r="H121" s="153" t="s">
+      <c r="H121" s="151" t="s">
         <v>93</v>
       </c>
       <c r="I121" s="35"/>
       <c r="J121" s="36">
         <v>5</v>
       </c>
-      <c r="K121" s="159">
+      <c r="K121" s="157">
         <v>10</v>
       </c>
-      <c r="L121" s="160"/>
-      <c r="M121" s="160"/>
+      <c r="L121" s="158"/>
+      <c r="M121" s="158"/>
       <c r="N121" s="35"/>
-      <c r="O121" s="145"/>
-      <c r="P121" s="141"/>
-      <c r="Q121" s="153" t="s">
+      <c r="O121" s="144"/>
+      <c r="P121" s="140"/>
+      <c r="Q121" s="151" t="s">
         <v>264</v>
       </c>
       <c r="R121" s="63"/>
       <c r="S121" s="26"/>
     </row>
     <row r="122" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="200"/>
-      <c r="B122" s="166"/>
-      <c r="C122" s="229"/>
-      <c r="D122" s="230"/>
-      <c r="E122" s="152" t="s">
+      <c r="A122" s="198"/>
+      <c r="B122" s="164"/>
+      <c r="C122" s="227"/>
+      <c r="D122" s="228"/>
+      <c r="E122" s="150" t="s">
         <v>365</v>
       </c>
-      <c r="F122" s="155" t="s">
+      <c r="F122" s="153" t="s">
         <v>143</v>
       </c>
       <c r="G122" s="35" t="s">
         <v>366</v>
       </c>
-      <c r="H122" s="153" t="s">
+      <c r="H122" s="151" t="s">
         <v>93</v>
       </c>
       <c r="I122" s="35"/>
       <c r="J122" s="36">
         <v>5</v>
       </c>
-      <c r="K122" s="160"/>
-      <c r="L122" s="160"/>
-      <c r="M122" s="160"/>
+      <c r="K122" s="158"/>
+      <c r="L122" s="158"/>
+      <c r="M122" s="158"/>
       <c r="N122" s="35"/>
-      <c r="O122" s="153"/>
-      <c r="P122" s="155"/>
-      <c r="Q122" s="153" t="s">
+      <c r="O122" s="151"/>
+      <c r="P122" s="153"/>
+      <c r="Q122" s="151" t="s">
         <v>264</v>
       </c>
       <c r="R122" s="63"/>
       <c r="S122" s="26"/>
     </row>
     <row r="123" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="200"/>
-      <c r="B123" s="166"/>
-      <c r="C123" s="229"/>
-      <c r="D123" s="230"/>
-      <c r="E123" s="152" t="s">
+      <c r="A123" s="198"/>
+      <c r="B123" s="164"/>
+      <c r="C123" s="227"/>
+      <c r="D123" s="228"/>
+      <c r="E123" s="150" t="s">
         <v>364</v>
       </c>
-      <c r="F123" s="155" t="s">
+      <c r="F123" s="153" t="s">
         <v>143</v>
       </c>
       <c r="G123" s="35" t="s">
         <v>367</v>
       </c>
-      <c r="H123" s="153" t="s">
+      <c r="H123" s="151" t="s">
         <v>93</v>
       </c>
       <c r="I123" s="35"/>
       <c r="J123" s="36">
         <v>5</v>
       </c>
-      <c r="K123" s="161"/>
-      <c r="L123" s="160"/>
-      <c r="M123" s="160"/>
+      <c r="K123" s="159"/>
+      <c r="L123" s="158"/>
+      <c r="M123" s="158"/>
       <c r="N123" s="35"/>
-      <c r="O123" s="153"/>
-      <c r="P123" s="155"/>
-      <c r="Q123" s="153" t="s">
+      <c r="O123" s="151"/>
+      <c r="P123" s="153"/>
+      <c r="Q123" s="151" t="s">
         <v>264</v>
       </c>
       <c r="R123" s="63"/>
       <c r="S123" s="26"/>
     </row>
     <row r="124" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="200"/>
-      <c r="B124" s="166"/>
-      <c r="C124" s="223" t="s">
+      <c r="A124" s="198"/>
+      <c r="B124" s="164"/>
+      <c r="C124" s="221" t="s">
         <v>308</v>
       </c>
-      <c r="D124" s="224" t="s">
+      <c r="D124" s="222" t="s">
         <v>309</v>
       </c>
-      <c r="E124" s="224" t="s">
+      <c r="E124" s="222" t="s">
         <v>309</v>
       </c>
-      <c r="F124" s="150" t="s">
+      <c r="F124" s="148" t="s">
         <v>143</v>
       </c>
-      <c r="G124" s="145" t="s">
+      <c r="G124" s="144" t="s">
         <v>310</v>
       </c>
-      <c r="H124" s="153" t="s">
+      <c r="H124" s="151" t="s">
         <v>93</v>
       </c>
       <c r="I124" s="35"/>
@@ -7798,34 +7870,34 @@
       <c r="K124" s="36">
         <v>5</v>
       </c>
-      <c r="L124" s="222">
-        <v>5</v>
-      </c>
-      <c r="M124" s="160"/>
+      <c r="L124" s="220">
+        <v>5</v>
+      </c>
+      <c r="M124" s="158"/>
       <c r="N124" s="35"/>
-      <c r="O124" s="145"/>
-      <c r="P124" s="141"/>
+      <c r="O124" s="144"/>
+      <c r="P124" s="140"/>
       <c r="Q124" s="35"/>
       <c r="R124" s="63"/>
       <c r="S124" s="26"/>
     </row>
     <row r="125" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="200"/>
-      <c r="B125" s="166"/>
-      <c r="C125" s="225"/>
-      <c r="D125" s="224" t="s">
+      <c r="A125" s="198"/>
+      <c r="B125" s="164"/>
+      <c r="C125" s="223"/>
+      <c r="D125" s="222" t="s">
         <v>311</v>
       </c>
-      <c r="E125" s="224" t="s">
+      <c r="E125" s="222" t="s">
         <v>311</v>
       </c>
-      <c r="F125" s="150" t="s">
+      <c r="F125" s="148" t="s">
         <v>143</v>
       </c>
-      <c r="G125" s="145" t="s">
+      <c r="G125" s="144" t="s">
         <v>312</v>
       </c>
-      <c r="H125" s="153" t="s">
+      <c r="H125" s="151" t="s">
         <v>93</v>
       </c>
       <c r="I125" s="35"/>
@@ -7835,37 +7907,43 @@
       <c r="K125" s="36">
         <v>5</v>
       </c>
-      <c r="L125" s="160"/>
-      <c r="M125" s="160"/>
+      <c r="L125" s="158"/>
+      <c r="M125" s="158"/>
       <c r="N125" s="35"/>
-      <c r="O125" s="145"/>
-      <c r="P125" s="141"/>
+      <c r="O125" s="144"/>
+      <c r="P125" s="140"/>
       <c r="Q125" s="35"/>
       <c r="R125" s="63"/>
       <c r="S125" s="26"/>
     </row>
     <row r="126" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="200"/>
-      <c r="B126" s="166" t="s">
+      <c r="A126" s="198"/>
+      <c r="B126" s="164" t="s">
         <v>36</v>
       </c>
-      <c r="C126" s="162" t="s">
+      <c r="C126" s="160" t="s">
         <v>36</v>
       </c>
-      <c r="D126" s="146" t="s">
+      <c r="D126" s="145" t="s">
         <v>335</v>
       </c>
-      <c r="E126" s="142" t="s">
+      <c r="E126" s="141" t="s">
         <v>4</v>
       </c>
       <c r="F126" s="49"/>
       <c r="G126" s="41"/>
       <c r="H126" s="35"/>
       <c r="I126" s="35"/>
-      <c r="J126" s="36"/>
-      <c r="K126" s="36"/>
-      <c r="L126" s="36"/>
-      <c r="M126" s="159">
+      <c r="J126" s="36">
+        <v>5</v>
+      </c>
+      <c r="K126" s="36">
+        <v>5</v>
+      </c>
+      <c r="L126" s="157">
+        <v>5</v>
+      </c>
+      <c r="M126" s="157">
         <v>6</v>
       </c>
       <c r="N126" s="35"/>
@@ -7874,53 +7952,57 @@
       <c r="Q126" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="R126" s="156" t="s">
+      <c r="R126" s="154" t="s">
         <v>336</v>
       </c>
       <c r="S126" s="26"/>
     </row>
     <row r="127" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="200"/>
-      <c r="B127" s="166"/>
-      <c r="C127" s="174"/>
-      <c r="D127" s="146" t="s">
+      <c r="A127" s="198"/>
+      <c r="B127" s="164"/>
+      <c r="C127" s="172"/>
+      <c r="D127" s="145" t="s">
         <v>334</v>
       </c>
-      <c r="E127" s="142"/>
-      <c r="F127" s="141"/>
-      <c r="G127" s="145"/>
+      <c r="E127" s="141"/>
+      <c r="F127" s="140"/>
+      <c r="G127" s="144"/>
       <c r="H127" s="35"/>
       <c r="I127" s="35"/>
-      <c r="J127" s="36"/>
-      <c r="K127" s="36"/>
-      <c r="L127" s="36"/>
-      <c r="M127" s="160"/>
+      <c r="J127" s="36">
+        <v>5</v>
+      </c>
+      <c r="K127" s="36">
+        <v>5</v>
+      </c>
+      <c r="L127" s="159"/>
+      <c r="M127" s="158"/>
       <c r="N127" s="35"/>
-      <c r="O127" s="145"/>
-      <c r="P127" s="141"/>
+      <c r="O127" s="144"/>
+      <c r="P127" s="140"/>
       <c r="Q127" s="35"/>
-      <c r="R127" s="157"/>
+      <c r="R127" s="155"/>
       <c r="S127" s="26"/>
     </row>
     <row r="128" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="200"/>
-      <c r="B128" s="158" t="s">
+      <c r="A128" s="198"/>
+      <c r="B128" s="156" t="s">
         <v>351</v>
       </c>
-      <c r="C128" s="158" t="s">
+      <c r="C128" s="156" t="s">
         <v>351</v>
       </c>
-      <c r="D128" s="152" t="s">
+      <c r="D128" s="150" t="s">
         <v>338</v>
       </c>
-      <c r="E128" s="152" t="s">
+      <c r="E128" s="150" t="s">
         <v>338</v>
       </c>
-      <c r="F128" s="155" t="s">
+      <c r="F128" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G128" s="153"/>
-      <c r="H128" s="153" t="s">
+      <c r="G128" s="151"/>
+      <c r="H128" s="151" t="s">
         <v>93</v>
       </c>
       <c r="I128" s="35"/>
@@ -7930,36 +8012,36 @@
       <c r="K128" s="36">
         <v>7</v>
       </c>
-      <c r="L128" s="159">
-        <v>5</v>
-      </c>
-      <c r="M128" s="159">
+      <c r="L128" s="157">
+        <v>5</v>
+      </c>
+      <c r="M128" s="157">
         <v>7</v>
       </c>
       <c r="N128" s="35"/>
       <c r="O128" s="35"/>
-      <c r="P128" s="154"/>
+      <c r="P128" s="152"/>
       <c r="Q128" s="35" t="s">
         <v>342</v>
       </c>
-      <c r="R128" s="233"/>
+      <c r="R128" s="231"/>
       <c r="S128" s="26"/>
     </row>
     <row r="129" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="200"/>
-      <c r="B129" s="158"/>
-      <c r="C129" s="158"/>
-      <c r="D129" s="152" t="s">
+      <c r="A129" s="198"/>
+      <c r="B129" s="156"/>
+      <c r="C129" s="156"/>
+      <c r="D129" s="150" t="s">
         <v>339</v>
       </c>
-      <c r="E129" s="152" t="s">
+      <c r="E129" s="150" t="s">
         <v>339</v>
       </c>
-      <c r="F129" s="155" t="s">
+      <c r="F129" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G129" s="153"/>
-      <c r="H129" s="153" t="s">
+      <c r="G129" s="151"/>
+      <c r="H129" s="151" t="s">
         <v>93</v>
       </c>
       <c r="I129" s="35"/>
@@ -7969,32 +8051,32 @@
       <c r="K129" s="36">
         <v>3</v>
       </c>
-      <c r="L129" s="160"/>
-      <c r="M129" s="160"/>
+      <c r="L129" s="158"/>
+      <c r="M129" s="158"/>
       <c r="N129" s="35"/>
       <c r="O129" s="35"/>
-      <c r="P129" s="154"/>
+      <c r="P129" s="152"/>
       <c r="Q129" s="35" t="s">
         <v>342</v>
       </c>
-      <c r="R129" s="233"/>
+      <c r="R129" s="231"/>
       <c r="S129" s="26"/>
     </row>
     <row r="130" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="200"/>
-      <c r="B130" s="158"/>
-      <c r="C130" s="158"/>
-      <c r="D130" s="152" t="s">
+      <c r="A130" s="198"/>
+      <c r="B130" s="156"/>
+      <c r="C130" s="156"/>
+      <c r="D130" s="150" t="s">
         <v>340</v>
       </c>
-      <c r="E130" s="152" t="s">
+      <c r="E130" s="150" t="s">
         <v>340</v>
       </c>
-      <c r="F130" s="155" t="s">
+      <c r="F130" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G130" s="153"/>
-      <c r="H130" s="153" t="s">
+      <c r="G130" s="151"/>
+      <c r="H130" s="151" t="s">
         <v>93</v>
       </c>
       <c r="I130" s="35"/>
@@ -8004,46 +8086,46 @@
       <c r="K130" s="36">
         <v>7</v>
       </c>
-      <c r="L130" s="160"/>
-      <c r="M130" s="160"/>
+      <c r="L130" s="158"/>
+      <c r="M130" s="158"/>
       <c r="N130" s="35"/>
       <c r="O130" s="35"/>
-      <c r="P130" s="154"/>
+      <c r="P130" s="152"/>
       <c r="Q130" s="35" t="s">
         <v>342</v>
       </c>
-      <c r="R130" s="233"/>
+      <c r="R130" s="231"/>
       <c r="S130" s="26"/>
     </row>
     <row r="131" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="200"/>
-      <c r="B131" s="158"/>
-      <c r="C131" s="158"/>
-      <c r="D131" s="152" t="s">
+      <c r="A131" s="198"/>
+      <c r="B131" s="156"/>
+      <c r="C131" s="156"/>
+      <c r="D131" s="150" t="s">
         <v>341</v>
       </c>
-      <c r="E131" s="152" t="s">
+      <c r="E131" s="150" t="s">
         <v>341</v>
       </c>
-      <c r="F131" s="155" t="s">
+      <c r="F131" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G131" s="153"/>
-      <c r="H131" s="153" t="s">
+      <c r="G131" s="151"/>
+      <c r="H131" s="151" t="s">
         <v>93</v>
       </c>
-      <c r="I131" s="153"/>
+      <c r="I131" s="151"/>
       <c r="J131" s="53">
         <v>5</v>
       </c>
       <c r="K131" s="53">
         <v>7</v>
       </c>
-      <c r="L131" s="160"/>
-      <c r="M131" s="160"/>
-      <c r="N131" s="153"/>
-      <c r="O131" s="153"/>
-      <c r="P131" s="155"/>
+      <c r="L131" s="158"/>
+      <c r="M131" s="158"/>
+      <c r="N131" s="151"/>
+      <c r="O131" s="151"/>
+      <c r="P131" s="153"/>
       <c r="Q131" s="35" t="s">
         <v>342</v>
       </c>
@@ -8051,42 +8133,42 @@
       <c r="S131" s="15"/>
     </row>
     <row r="132" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="200"/>
-      <c r="B132" s="158" t="s">
+      <c r="A132" s="198"/>
+      <c r="B132" s="156" t="s">
         <v>352</v>
       </c>
-      <c r="C132" s="158" t="s">
+      <c r="C132" s="156" t="s">
         <v>352</v>
       </c>
-      <c r="D132" s="152" t="s">
+      <c r="D132" s="150" t="s">
         <v>353</v>
       </c>
-      <c r="E132" s="152" t="s">
+      <c r="E132" s="150" t="s">
         <v>353</v>
       </c>
-      <c r="F132" s="155" t="s">
+      <c r="F132" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G132" s="153"/>
-      <c r="H132" s="153" t="s">
+      <c r="G132" s="151"/>
+      <c r="H132" s="151" t="s">
         <v>93</v>
       </c>
-      <c r="I132" s="153"/>
+      <c r="I132" s="151"/>
       <c r="J132" s="53">
         <v>5</v>
       </c>
       <c r="K132" s="53">
         <v>10</v>
       </c>
-      <c r="L132" s="179">
-        <v>5</v>
-      </c>
-      <c r="M132" s="179">
+      <c r="L132" s="177">
+        <v>5</v>
+      </c>
+      <c r="M132" s="177">
         <v>9</v>
       </c>
-      <c r="N132" s="153"/>
-      <c r="O132" s="153"/>
-      <c r="P132" s="155"/>
+      <c r="N132" s="151"/>
+      <c r="O132" s="151"/>
+      <c r="P132" s="153"/>
       <c r="Q132" s="35" t="s">
         <v>342</v>
       </c>
@@ -8094,34 +8176,34 @@
       <c r="S132" s="15"/>
     </row>
     <row r="133" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="200"/>
-      <c r="B133" s="158"/>
-      <c r="C133" s="158"/>
-      <c r="D133" s="152" t="s">
+      <c r="A133" s="198"/>
+      <c r="B133" s="156"/>
+      <c r="C133" s="156"/>
+      <c r="D133" s="150" t="s">
         <v>354</v>
       </c>
-      <c r="E133" s="152" t="s">
+      <c r="E133" s="150" t="s">
         <v>354</v>
       </c>
-      <c r="F133" s="155" t="s">
+      <c r="F133" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G133" s="153"/>
-      <c r="H133" s="153" t="s">
+      <c r="G133" s="151"/>
+      <c r="H133" s="151" t="s">
         <v>93</v>
       </c>
-      <c r="I133" s="153"/>
+      <c r="I133" s="151"/>
       <c r="J133" s="53">
         <v>5</v>
       </c>
       <c r="K133" s="53">
         <v>4</v>
       </c>
-      <c r="L133" s="234"/>
-      <c r="M133" s="234"/>
-      <c r="N133" s="153"/>
-      <c r="O133" s="153"/>
-      <c r="P133" s="155"/>
+      <c r="L133" s="232"/>
+      <c r="M133" s="232"/>
+      <c r="N133" s="151"/>
+      <c r="O133" s="151"/>
+      <c r="P133" s="153"/>
       <c r="Q133" s="35" t="s">
         <v>342</v>
       </c>
@@ -8129,34 +8211,34 @@
       <c r="S133" s="15"/>
     </row>
     <row r="134" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="201"/>
-      <c r="B134" s="158"/>
-      <c r="C134" s="158"/>
-      <c r="D134" s="152" t="s">
+      <c r="A134" s="199"/>
+      <c r="B134" s="156"/>
+      <c r="C134" s="156"/>
+      <c r="D134" s="150" t="s">
         <v>355</v>
       </c>
-      <c r="E134" s="152" t="s">
+      <c r="E134" s="150" t="s">
         <v>355</v>
       </c>
-      <c r="F134" s="155" t="s">
+      <c r="F134" s="153" t="s">
         <v>143</v>
       </c>
-      <c r="G134" s="153"/>
-      <c r="H134" s="153" t="s">
+      <c r="G134" s="151"/>
+      <c r="H134" s="151" t="s">
         <v>93</v>
       </c>
-      <c r="I134" s="153"/>
+      <c r="I134" s="151"/>
       <c r="J134" s="53">
         <v>5</v>
       </c>
       <c r="K134" s="53">
         <v>6</v>
       </c>
-      <c r="L134" s="235"/>
-      <c r="M134" s="235"/>
-      <c r="N134" s="153"/>
-      <c r="O134" s="153"/>
-      <c r="P134" s="155"/>
+      <c r="L134" s="233"/>
+      <c r="M134" s="233"/>
+      <c r="N134" s="151"/>
+      <c r="O134" s="151"/>
+      <c r="P134" s="153"/>
       <c r="Q134" s="35" t="s">
         <v>342</v>
       </c>
@@ -8172,15 +8254,15 @@
       <c r="G135" s="11"/>
       <c r="H135" s="11"/>
       <c r="I135" s="11"/>
-      <c r="J135" s="231"/>
-      <c r="K135" s="231"/>
-      <c r="L135" s="231"/>
-      <c r="M135" s="231"/>
+      <c r="J135" s="229"/>
+      <c r="K135" s="229"/>
+      <c r="L135" s="229"/>
+      <c r="M135" s="229"/>
       <c r="N135" s="11"/>
       <c r="O135" s="11"/>
       <c r="P135" s="31"/>
       <c r="Q135" s="11"/>
-      <c r="R135" s="232"/>
+      <c r="R135" s="230"/>
     </row>
     <row r="139" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C139" s="10"/>
@@ -8251,13 +8333,14 @@
       <c r="D150" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="104">
+  <mergeCells count="106">
     <mergeCell ref="M128:M131"/>
     <mergeCell ref="M132:M134"/>
     <mergeCell ref="D121:D123"/>
     <mergeCell ref="K121:K123"/>
     <mergeCell ref="L128:L131"/>
     <mergeCell ref="L132:L134"/>
+    <mergeCell ref="L126:L127"/>
     <mergeCell ref="B132:B134"/>
     <mergeCell ref="B128:B131"/>
     <mergeCell ref="A99:A134"/>
@@ -8265,6 +8348,7 @@
     <mergeCell ref="L119:L123"/>
     <mergeCell ref="C128:C131"/>
     <mergeCell ref="C132:C134"/>
+    <mergeCell ref="I100:M118"/>
     <mergeCell ref="K3:K6"/>
     <mergeCell ref="C3:C7"/>
     <mergeCell ref="C119:C123"/>
@@ -8435,10 +8519,10 @@
   <sheetData>
     <row r="5" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="3:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="210" t="s">
+      <c r="C6" s="208" t="s">
         <v>149</v>
       </c>
-      <c r="D6" s="211"/>
+      <c r="D6" s="209"/>
     </row>
     <row r="7" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C7" s="93" t="s">
@@ -8449,7 +8533,7 @@
       </c>
     </row>
     <row r="8" spans="3:4" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="C8" s="207" t="s">
+      <c r="C8" s="205" t="s">
         <v>294</v>
       </c>
       <c r="D8" s="89" t="s">
@@ -8457,19 +8541,19 @@
       </c>
     </row>
     <row r="9" spans="3:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="C9" s="208"/>
+      <c r="C9" s="206"/>
       <c r="D9" s="89" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="10" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C10" s="208"/>
+      <c r="C10" s="206"/>
       <c r="D10" s="89" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="11" spans="3:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="C11" s="209"/>
+      <c r="C11" s="207"/>
       <c r="D11" s="89" t="s">
         <v>290</v>
       </c>
@@ -8518,87 +8602,87 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="151" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="151" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="151" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" style="151" customWidth="1"/>
-    <col min="5" max="8" width="11" style="151" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="151"/>
+    <col min="1" max="1" width="11" style="149" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="149" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="149" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" style="149" customWidth="1"/>
+    <col min="5" max="8" width="11" style="149" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="149"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="149" t="s">
         <v>326</v>
       </c>
-      <c r="B1" s="151" t="s">
+      <c r="B1" s="149" t="s">
         <v>325</v>
       </c>
-      <c r="C1" s="151" t="s">
+      <c r="C1" s="149" t="s">
         <v>329</v>
       </c>
-      <c r="D1" s="151" t="s">
+      <c r="D1" s="149" t="s">
         <v>324</v>
       </c>
-      <c r="E1" s="151" t="s">
+      <c r="E1" s="149" t="s">
         <v>320</v>
       </c>
-      <c r="F1" s="151" t="s">
+      <c r="F1" s="149" t="s">
         <v>321</v>
       </c>
-      <c r="G1" s="151" t="s">
+      <c r="G1" s="149" t="s">
         <v>322</v>
       </c>
-      <c r="H1" s="151" t="s">
+      <c r="H1" s="149" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="151">
+      <c r="A2" s="149">
         <v>1</v>
       </c>
-      <c r="B2" s="151" t="s">
+      <c r="B2" s="149" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="151" t="s">
+      <c r="C2" s="149" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="151">
+      <c r="A3" s="149">
         <v>2</v>
       </c>
-      <c r="B3" s="151" t="s">
+      <c r="B3" s="149" t="s">
         <v>318</v>
       </c>
-      <c r="C3" s="151" t="s">
+      <c r="C3" s="149" t="s">
         <v>331</v>
       </c>
-      <c r="D3" s="151" t="s">
+      <c r="D3" s="149" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="151">
+      <c r="A4" s="149">
         <v>3</v>
       </c>
-      <c r="B4" s="151" t="s">
+      <c r="B4" s="149" t="s">
         <v>328</v>
       </c>
-      <c r="C4" s="151" t="s">
+      <c r="C4" s="149" t="s">
         <v>332</v>
       </c>
-      <c r="D4" s="151" t="s">
+      <c r="D4" s="149" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="151">
+      <c r="A5" s="149">
         <v>4</v>
       </c>
-      <c r="B5" s="151" t="s">
+      <c r="B5" s="149" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="151" t="s">
+      <c r="D5" s="149" t="s">
         <v>333</v>
       </c>
     </row>

</xml_diff>